<commit_message>
First draft with structure and figures from screenshots
</commit_message>
<xml_diff>
--- a/KES-MPS.xlsx
+++ b/KES-MPS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Brent" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,12 +21,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
   <si>
     <t xml:space="preserve">Simulation results</t>
   </si>
   <si>
-    <t xml:space="preserve">NoTOF 1-8 MeV</t>
+    <t xml:space="preserve">NoTOF 3-6 MeV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOF 1-8 MeV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prototypes</t>
   </si>
   <si>
     <t xml:space="preserve">MPS</t>
@@ -35,12 +41,6 @@
     <t xml:space="preserve">KES</t>
   </si>
   <si>
-    <t xml:space="preserve">MPS 1-8 MeV TOF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KES 3-6 MeV no TOF</t>
-  </si>
-  <si>
     <t xml:space="preserve">d1 (mm)</t>
   </si>
   <si>
@@ -89,10 +89,10 @@
     <t xml:space="preserve">** Efficiency at the center of the camera</t>
   </si>
   <si>
-    <t xml:space="preserve">MPS, NoTOF, 1 MeV &lt; E &lt; 8 MeV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KES, NoTOF, 1 MeV &lt; E &lt; 8 MeV</t>
+    <t xml:space="preserve">MPS, TOF, 1 MeV &lt; E &lt; 8 MeV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KES, TOF, 1 MeV &lt; E &lt; 8 MeV</t>
   </si>
   <si>
     <t xml:space="preserve">Geometrical calculations</t>
@@ -188,7 +188,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -202,6 +202,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -237,16 +241,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>432720</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>61200</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>82080</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>53640</xdr:rowOff>
+      <xdr:rowOff>53280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -260,7 +264,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9814680" y="0"/>
-          <a:ext cx="1973520" cy="2979720"/>
+          <a:ext cx="1973160" cy="2979360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -274,16 +278,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>47160</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>256680</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>56160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>551880</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>180000</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>21600</xdr:rowOff>
+      <xdr:rowOff>21240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -297,7 +301,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7686000" y="56160"/>
-          <a:ext cx="2247840" cy="2891520"/>
+          <a:ext cx="2247480" cy="2891160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -312,15 +316,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>176400</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>111600</xdr:rowOff>
+      <xdr:colOff>207000</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>37800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>112680</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>72360</xdr:rowOff>
+      <xdr:colOff>142920</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>160920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -333,8 +337,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="176400" y="3037680"/>
-          <a:ext cx="4079520" cy="5000040"/>
+          <a:off x="207000" y="3288960"/>
+          <a:ext cx="4079160" cy="4999680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -348,16 +352,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>230040</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>439560</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>149400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>191880</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>401400</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>89280</xdr:rowOff>
+      <xdr:rowOff>88920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -371,7 +375,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11936160" y="474480"/>
-          <a:ext cx="4029120" cy="1890360"/>
+          <a:ext cx="4028760" cy="1890000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -391,10 +395,10 @@
       <xdr:rowOff>73800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>265320</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>474480</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>106560</xdr:rowOff>
+      <xdr:rowOff>106200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -408,7 +412,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5113440" y="3650040"/>
-          <a:ext cx="4533840" cy="3771720"/>
+          <a:ext cx="4533480" cy="3771360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -422,16 +426,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>376200</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>4680</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>77040</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>286200</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>8640</xdr:rowOff>
+      <xdr:rowOff>8280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -445,7 +449,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10339200" y="3576240"/>
-          <a:ext cx="4349160" cy="3747600"/>
+          <a:ext cx="4348800" cy="3747240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -471,9 +475,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>523080</xdr:colOff>
+      <xdr:colOff>522720</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>53640</xdr:rowOff>
+      <xdr:rowOff>53280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -487,7 +491,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5694120" y="0"/>
-          <a:ext cx="1993320" cy="2979720"/>
+          <a:ext cx="1992960" cy="2979360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -508,9 +512,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>235440</xdr:colOff>
+      <xdr:colOff>235080</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>128160</xdr:rowOff>
+      <xdr:rowOff>127800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -524,7 +528,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3999960" y="0"/>
-          <a:ext cx="2238120" cy="2891520"/>
+          <a:ext cx="2237760" cy="2891160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -545,9 +549,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>120240</xdr:colOff>
+      <xdr:colOff>119880</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>31680</xdr:rowOff>
+      <xdr:rowOff>31320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -561,7 +565,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7904520" y="416880"/>
-          <a:ext cx="4028400" cy="1890360"/>
+          <a:ext cx="4028040" cy="1890000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -581,285 +585,338 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q21"/>
+  <dimension ref="A2:Q21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="3.10714285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="11.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="3.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.23"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="2"/>
-    </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="2"/>
+      <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="3"/>
+      <c r="E2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="1"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="H3" s="3"/>
+      <c r="I3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="0" t="s">
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="D4" s="1"/>
+      <c r="E4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="n">
+      <c r="B5" s="5" t="n">
         <v>304</v>
       </c>
-      <c r="C4" s="4" t="n">
+      <c r="C5" s="5" t="n">
         <v>250</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="4" t="n">
-        <v>180</v>
-      </c>
-      <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" s="4" t="n">
-        <v>200</v>
-      </c>
+      <c r="A6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>180</v>
+      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="4" t="n">
-        <f aca="false">B4+B5+B6</f>
-        <v>484</v>
-      </c>
-      <c r="C7" s="4" t="n">
-        <f aca="false">SUM(C4:C6)</f>
-        <v>450</v>
+      <c r="A7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>200</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="4" t="n">
-        <v>5.4</v>
-      </c>
-      <c r="C8" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="A8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="5" t="n">
+        <f aca="false">B5+B6+B7</f>
+        <v>484</v>
+      </c>
+      <c r="C8" s="5" t="n">
+        <f aca="false">SUM(C5:C7)</f>
+        <v>450</v>
+      </c>
+      <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="A9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="5" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="4" t="n">
-        <f aca="false">2.6/8</f>
-        <v>0.325</v>
-      </c>
+      <c r="A10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="5"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="5" t="n">
+        <f aca="false">2.6/8</f>
+        <v>0.325</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="4" t="n">
-        <f aca="false">B5*B10</f>
+      <c r="B12" s="5" t="n">
+        <f aca="false">B6*B11</f>
         <v>58.5</v>
       </c>
-      <c r="C11" s="4" t="n">
+      <c r="C12" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1" t="n">
+      <c r="D12" s="1"/>
+      <c r="E12" s="1" t="n">
         <f aca="false">180*0.4</f>
         <v>72</v>
       </c>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
+      <c r="F12" s="1"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="4" t="n">
-        <f aca="false">B8*(1+B4/B5)</f>
+      <c r="B13" s="5" t="n">
+        <f aca="false">B9*(1+B5/B6)</f>
         <v>14.52</v>
       </c>
-      <c r="C12" s="4" t="n">
-        <f aca="false">C8*(1+C4/C6)</f>
+      <c r="C13" s="5" t="n">
+        <f aca="false">C9*(1+C5/C7)</f>
         <v>13.5</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="5" t="n">
-        <f aca="false">B8/(B7*B5)*(1-B10)</f>
-        <v>4.18388429752066E-005</v>
-      </c>
-      <c r="C13" s="5" t="n">
-        <f aca="false">C8/(C7*C6)</f>
-        <v>6.66666666666667E-005</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="6" t="n">
+        <f aca="false">B9/(B8*B6)*(1-B11)</f>
+        <v>4.18388429752066E-005</v>
+      </c>
+      <c r="C14" s="6" t="n">
+        <f aca="false">C9/(C8*C7)</f>
+        <v>6.66666666666667E-005</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="4" t="n">
-        <v>400</v>
-      </c>
-      <c r="F14" s="4" t="n">
-        <v>700</v>
-      </c>
-      <c r="G14" s="0" t="n">
-        <v>400</v>
-      </c>
-      <c r="H14" s="0" t="n">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="4" t="n">
-        <f aca="false">C13/B13</f>
-        <v>1.59341563786008</v>
-      </c>
+      <c r="B15" s="5"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="4" t="n">
-        <f aca="false">F14/E14</f>
+      <c r="E15" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>350</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>400</v>
+      </c>
+      <c r="H15" s="1" t="n">
+        <v>700</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="5" t="n">
+        <f aca="false">C14/B14</f>
+        <v>1.59341563786008</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="5" t="n">
+        <f aca="false">F15/E15</f>
         <v>1.75</v>
       </c>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="s">
+      <c r="F16" s="5"/>
+      <c r="G16" s="5" t="n">
+        <f aca="false">H15/G15</f>
+        <v>1.75</v>
+      </c>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5" t="n">
+        <f aca="false">J15/I15</f>
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6" t="s">
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I21" s="7" t="s">
+      <c r="I21" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="Q21" s="7" t="s">
+      <c r="Q21" s="8" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="A17:E17"/>
+  <mergeCells count="6">
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
     <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A19:E19"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -875,17 +932,17 @@
   </sheetPr>
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="1" sqref="I16 D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.7142857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="3.10714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="3.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -904,89 +961,89 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>3</v>
+      <c r="C3" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="n">
+      <c r="B4" s="5" t="n">
         <v>300</v>
       </c>
-      <c r="C4" s="4" t="n">
+      <c r="C4" s="5" t="n">
         <v>300</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4" t="n">
+      <c r="B5" s="5" t="n">
         <v>200</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4" t="n">
+      <c r="B6" s="5" t="n">
         <v>300</v>
       </c>
-      <c r="C6" s="4" t="n">
+      <c r="C6" s="5" t="n">
         <v>300</v>
       </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="4" t="n">
+      <c r="B7" s="5" t="n">
         <f aca="false">B4+B5+B6</f>
         <v>800</v>
       </c>
-      <c r="C7" s="4" t="n">
+      <c r="C7" s="5" t="n">
         <f aca="false">SUM(C4:C6)</f>
         <v>600</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="4" t="n">
+      <c r="B8" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="C8" s="4" t="n">
+      <c r="C8" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="4" t="n">
+      <c r="B9" s="5" t="n">
         <v>2</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="4" t="n">
+      <c r="B10" s="5" t="n">
         <f aca="false">B9/(B8+B9)</f>
         <v>0.5</v>
       </c>
@@ -994,48 +1051,48 @@
       <c r="D10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="4" t="n">
+      <c r="B11" s="5" t="n">
         <f aca="false">B5*B10</f>
         <v>100</v>
       </c>
-      <c r="C11" s="4" t="n">
+      <c r="C11" s="5" t="n">
         <v>40</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="4" t="n">
+      <c r="B12" s="5" t="n">
         <f aca="false">B8*(1+B4/B5)</f>
         <v>5</v>
       </c>
-      <c r="C12" s="4" t="n">
+      <c r="C12" s="5" t="n">
         <f aca="false">C8*(1+C4/C6)</f>
         <v>12</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="5" t="n">
+      <c r="B13" s="6" t="n">
         <f aca="false">B8*(1-B10)/(B7*B5)</f>
         <v>6.25E-006</v>
       </c>
-      <c r="C13" s="5" t="n">
+      <c r="C13" s="6" t="n">
         <f aca="false">C8/(C7*C6)</f>
         <v>3.33333333333333E-005</v>
       </c>
-      <c r="D13" s="4"/>
+      <c r="D13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="1"/>
@@ -1043,10 +1100,10 @@
       <c r="D14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="4" t="n">
+      <c r="B15" s="5" t="n">
         <f aca="false">C13/B13</f>
         <v>5.33333333333333</v>
       </c>
@@ -1054,20 +1111,20 @@
       <c r="D15" s="1"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1077,7 +1134,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
Etienne's update with subtantial changes...
</commit_message>
<xml_diff>
--- a/KES-MPS.xlsx
+++ b/KES-MPS.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
   <si>
     <t xml:space="preserve">Simulation results</t>
   </si>
@@ -83,10 +83,19 @@
     <t xml:space="preserve">KES eff/ MPS eff</t>
   </si>
   <si>
+    <t xml:space="preserve">KES Det. unit FOV / MPS</t>
+  </si>
+  <si>
     <t xml:space="preserve">* no KES transparency taken into account</t>
   </si>
   <si>
+    <t xml:space="preserve">µ (mm-1)</t>
+  </si>
+  <si>
     <t xml:space="preserve">** Efficiency at the center of the camera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se (mm)</t>
   </si>
   <si>
     <t xml:space="preserve">MPS, TOF, 1 MeV &lt; E &lt; 8 MeV</t>
@@ -205,7 +214,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -248,9 +257,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>291240</xdr:colOff>
+      <xdr:colOff>290160</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>53280</xdr:rowOff>
+      <xdr:rowOff>52200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -263,8 +272,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9814680" y="0"/>
-          <a:ext cx="1973160" cy="2979360"/>
+          <a:off x="9776520" y="0"/>
+          <a:ext cx="2029320" cy="2978280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -285,9 +294,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>180000</xdr:colOff>
+      <xdr:colOff>178920</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>21240</xdr:rowOff>
+      <xdr:rowOff>20160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -300,8 +309,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7686000" y="56160"/>
-          <a:ext cx="2247480" cy="2891160"/>
+          <a:off x="7571880" y="56160"/>
+          <a:ext cx="2322360" cy="2890080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -322,9 +331,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>142920</xdr:colOff>
+      <xdr:colOff>141840</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>160920</xdr:rowOff>
+      <xdr:rowOff>159840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -338,7 +347,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="207000" y="3288960"/>
-          <a:ext cx="4079160" cy="4999680"/>
+          <a:ext cx="4001760" cy="4998600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -359,9 +368,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>401400</xdr:colOff>
+      <xdr:colOff>400320</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>88920</xdr:rowOff>
+      <xdr:rowOff>87840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -374,8 +383,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11936160" y="474480"/>
-          <a:ext cx="4028760" cy="1890000"/>
+          <a:off x="11955240" y="474480"/>
+          <a:ext cx="4161240" cy="1888920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -396,9 +405,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>474480</xdr:colOff>
+      <xdr:colOff>473400</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>106200</xdr:rowOff>
+      <xdr:rowOff>105120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -411,8 +420,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5113440" y="3650040"/>
-          <a:ext cx="4533480" cy="3771360"/>
+          <a:off x="5018040" y="3650040"/>
+          <a:ext cx="4570560" cy="3770280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -433,9 +442,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>286200</xdr:colOff>
+      <xdr:colOff>285120</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>8280</xdr:rowOff>
+      <xdr:rowOff>7200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -448,8 +457,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10339200" y="3576240"/>
-          <a:ext cx="4348800" cy="3747240"/>
+          <a:off x="10320120" y="3576240"/>
+          <a:ext cx="4480920" cy="3746160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -475,9 +484,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>522720</xdr:colOff>
+      <xdr:colOff>521640</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>53280</xdr:rowOff>
+      <xdr:rowOff>52200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -490,8 +499,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5694120" y="0"/>
-          <a:ext cx="1992960" cy="2979360"/>
+          <a:off x="5663520" y="0"/>
+          <a:ext cx="2049480" cy="2978280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -512,9 +521,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>235080</xdr:colOff>
+      <xdr:colOff>234000</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>127800</xdr:rowOff>
+      <xdr:rowOff>126720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -527,8 +536,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3999960" y="0"/>
-          <a:ext cx="2237760" cy="2891160"/>
+          <a:off x="3912120" y="0"/>
+          <a:ext cx="2313000" cy="2890080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -549,9 +558,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>119880</xdr:colOff>
+      <xdr:colOff>118800</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>30240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -564,8 +573,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7904520" y="416880"/>
-          <a:ext cx="4028040" cy="1890000"/>
+          <a:off x="7950240" y="416880"/>
+          <a:ext cx="4160520" cy="1888920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -585,22 +594,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:Q21"/>
+  <dimension ref="A2:X21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="11.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="3.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.51"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -807,6 +816,12 @@
       <c r="F13" s="1"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
+      <c r="I13" s="0" t="n">
+        <v>17.5</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>15.6</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
@@ -879,30 +894,61 @@
         <v>0.875</v>
       </c>
     </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <f aca="false">C13/B13</f>
+        <v>0.929752066115703</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <f aca="false">J13/I13</f>
+        <v>0.891428571428571</v>
+      </c>
+    </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
+      <c r="U18" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="V18" s="0" t="n">
+        <f aca="false">4.4*10^(-2)*18/10</f>
+        <v>0.0792</v>
+      </c>
+      <c r="X18" s="0" t="n">
+        <f aca="false">EXP(-V18*5)</f>
+        <v>0.673006695937386</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
+      <c r="U19" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="V19" s="0" t="n">
+        <f aca="false">LN(2)/(V18*TAN(60*3.14159/180))</f>
+        <v>5.05289809045416</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I21" s="8" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="Q21" s="8" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -932,17 +978,17 @@
   </sheetPr>
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="1" sqref="I16 D8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="3.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -954,7 +1000,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1"/>
@@ -962,7 +1008,7 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>5</v>
@@ -1112,7 +1158,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -1120,7 +1166,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>

</xml_diff>

<commit_message>
Etienne's review up to the Results section
</commit_message>
<xml_diff>
--- a/KES-MPS.xlsx
+++ b/KES-MPS.xlsx
@@ -10,6 +10,7 @@
   <sheets>
     <sheet name="Brent" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Lin" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="AbsoluteEfficiency" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,11 +22,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="39">
   <si>
     <t xml:space="preserve">Simulation results</t>
   </si>
   <si>
+    <t xml:space="preserve">Priegnitz 2015</t>
+  </si>
+  <si>
     <t xml:space="preserve">NoTOF 3-6 MeV</t>
   </si>
   <si>
@@ -53,6 +57,9 @@
     <t xml:space="preserve">L (mm)</t>
   </si>
   <si>
+    <t xml:space="preserve">H (mm)</t>
+  </si>
+  <si>
     <t xml:space="preserve">s (mm)</t>
   </si>
   <si>
@@ -62,6 +69,18 @@
     <t xml:space="preserve">septa (mm)</t>
   </si>
   <si>
+    <t xml:space="preserve">w (detector width) (mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p (mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longueur caméra (mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nbre fentes</t>
+  </si>
+  <si>
     <t xml:space="preserve">f</t>
   </si>
   <si>
@@ -71,52 +90,66 @@
     <t xml:space="preserve">Det. Unit FOV (mm)</t>
   </si>
   <si>
+    <t xml:space="preserve">Det. Unit. Geom. Efficiency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Det. Unit efficiency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Det. Unit efficiency (published)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falloff amplitude (4 mm bin)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KES eff/ MPS eff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KES Det. unit FOV / MPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* no KES transparency taken into account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">µ (mm-1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">** Efficiency at the center of the camera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se (mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPS, TOF, 1 MeV &lt; E &lt; 8 MeV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KES, TOF, 1 MeV &lt; E &lt; 8 MeV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geometrical calculations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPS </t>
+  </si>
+  <si>
     <t xml:space="preserve">Lin. Coll. Eff (relative)</t>
   </si>
   <si>
-    <t xml:space="preserve">**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Falloff amplitude (4 mm bin)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KES eff/ MPS eff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KES Det. unit FOV / MPS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* no KES transparency taken into account</t>
-  </si>
-  <si>
-    <t xml:space="preserve">µ (mm-1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">** Efficiency at the center of the camera</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Se (mm)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MPS, TOF, 1 MeV &lt; E &lt; 8 MeV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KES, TOF, 1 MeV &lt; E &lt; 8 MeV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geometrical calculations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MPS </t>
+    <t xml:space="preserve">Detection efficiency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Efficaicté KES publiée</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.00E+000"/>
+    <numFmt numFmtId="165" formatCode="0.00E+00"/>
+    <numFmt numFmtId="166" formatCode="0.00E+000"/>
+    <numFmt numFmtId="167" formatCode="#,##0.00"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -148,12 +181,24 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF200"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -197,7 +242,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -214,6 +259,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -222,7 +271,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -243,6 +316,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFF200"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFCCCCCC"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -250,16 +383,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>61200</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>235800</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>290160</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>464400</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>52200</xdr:rowOff>
+      <xdr:rowOff>51840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -272,8 +405,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9776520" y="0"/>
-          <a:ext cx="2029320" cy="2978280"/>
+          <a:off x="9779760" y="0"/>
+          <a:ext cx="2030760" cy="2977920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -287,16 +420,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>256680</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>431280</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>56160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>178920</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>353160</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>20160</xdr:rowOff>
+      <xdr:rowOff>19800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -309,8 +442,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7571880" y="56160"/>
-          <a:ext cx="2322360" cy="2890080"/>
+          <a:off x="7572240" y="56160"/>
+          <a:ext cx="2324880" cy="2889720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -325,15 +458,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>207000</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>37800</xdr:rowOff>
+      <xdr:colOff>173880</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>102960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>141840</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>159840</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>282960</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>61920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -346,8 +479,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="207000" y="3288960"/>
-          <a:ext cx="4001760" cy="4998600"/>
+          <a:off x="173880" y="4492080"/>
+          <a:ext cx="4001400" cy="4998240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -362,15 +495,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>439560</xdr:colOff>
+      <xdr:colOff>13680</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>149400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>400320</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>574560</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>87840</xdr:rowOff>
+      <xdr:rowOff>87480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -383,8 +516,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11955240" y="474480"/>
-          <a:ext cx="4161240" cy="1888920"/>
+          <a:off x="11960280" y="474480"/>
+          <a:ext cx="4165200" cy="1888560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -398,16 +531,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>93960</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>73800</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>240480</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>106200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>473400</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>105120</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>363240</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>137520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -420,8 +553,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5018040" y="3650040"/>
-          <a:ext cx="4570560" cy="3770280"/>
+          <a:off x="4733640" y="4820400"/>
+          <a:ext cx="4572720" cy="3769920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -435,16 +568,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>4680</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>397080</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>54360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>285120</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>7200</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>76680</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>61200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -457,8 +590,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10320120" y="3576240"/>
-          <a:ext cx="4480920" cy="3746160"/>
+          <a:off x="9941040" y="4930920"/>
+          <a:ext cx="4485240" cy="3745800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -484,9 +617,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>521640</xdr:colOff>
+      <xdr:colOff>521280</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>52200</xdr:rowOff>
+      <xdr:rowOff>51840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -499,8 +632,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5663520" y="0"/>
-          <a:ext cx="2049480" cy="2978280"/>
+          <a:off x="5665320" y="0"/>
+          <a:ext cx="2050920" cy="2977920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -521,9 +654,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>234000</xdr:colOff>
+      <xdr:colOff>233640</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>126720</xdr:rowOff>
+      <xdr:rowOff>126360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -537,7 +670,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3912120" y="0"/>
-          <a:ext cx="2313000" cy="2890080"/>
+          <a:ext cx="2315160" cy="2889720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -558,9 +691,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>118800</xdr:colOff>
+      <xdr:colOff>118440</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>30240</xdr:rowOff>
+      <xdr:rowOff>29880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -573,8 +706,87 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7950240" y="416880"/>
-          <a:ext cx="4160520" cy="1888920"/>
+          <a:off x="7954920" y="416880"/>
+          <a:ext cx="4164120" cy="1888560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>34560</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>81360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>133200</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>17640</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Image 5" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8138880" y="3657600"/>
+          <a:ext cx="4162680" cy="1886760"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>416520</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>30960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>300960</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>155520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Image 2" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14210280" y="30960"/>
+          <a:ext cx="2323080" cy="2887920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -594,22 +806,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:X21"/>
+  <dimension ref="A2:X28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="3.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -627,328 +840,435 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="D3" s="1"/>
       <c r="E3" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" s="3"/>
-      <c r="G3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
+      <c r="C4" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="E4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="5" t="s">
+      <c r="F4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>5</v>
       </c>
+      <c r="H4" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="I4" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="5" t="n">
+      <c r="A5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="6" t="n">
         <v>304</v>
       </c>
-      <c r="C5" s="5" t="n">
+      <c r="C5" s="6" t="n">
         <v>250</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="5" t="n">
+      <c r="A6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="6" t="n">
         <v>180</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="5" t="n">
+      <c r="A7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="C7" s="5" t="n">
+      <c r="C7" s="6" t="n">
         <v>200</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="5" t="n">
+      <c r="A8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="6" t="n">
         <f aca="false">B5+B6+B7</f>
         <v>484</v>
       </c>
-      <c r="C8" s="5" t="n">
+      <c r="C8" s="6" t="n">
         <f aca="false">SUM(C5:C7)</f>
         <v>450</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="5" t="n">
-        <v>5.4</v>
-      </c>
-      <c r="C9" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="D9" s="5" t="s">
+      <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
+      <c r="B9" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="B10" s="6" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="C10" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="5" t="n">
-        <f aca="false">2.6/8</f>
-        <v>0.325</v>
-      </c>
+      <c r="A11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="6"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="5" t="n">
-        <f aca="false">B6*B11</f>
-        <v>58.5</v>
-      </c>
-      <c r="C12" s="5" t="n">
-        <v>40</v>
+      <c r="A12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="1" t="n">
-        <f aca="false">180*0.4</f>
-        <v>72</v>
-      </c>
+      <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="5" t="n">
-        <f aca="false">B9*(1+B5/B6)</f>
-        <v>14.52</v>
-      </c>
-      <c r="C13" s="5" t="n">
-        <f aca="false">C9*(1+C5/C7)</f>
-        <v>13.5</v>
-      </c>
+      <c r="A13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="7" t="n">
+        <f aca="false">B10+B11</f>
+        <v>5.4</v>
+      </c>
+      <c r="C13" s="7"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="0" t="n">
-        <v>17.5</v>
-      </c>
-      <c r="J13" s="0" t="n">
-        <v>15.6</v>
-      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="6" t="n">
-        <f aca="false">B9/(B8*B6)*(1-B11)</f>
-        <v>4.18388429752066E-005</v>
-      </c>
-      <c r="C14" s="6" t="n">
-        <f aca="false">C9/(C8*C7)</f>
-        <v>6.66666666666667E-005</v>
-      </c>
-      <c r="D14" s="5" t="s">
+      <c r="A14" s="7" t="s">
         <v>17</v>
       </c>
+      <c r="B14" s="7" t="n">
+        <v>25</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="1"/>
+      <c r="B15" s="7" t="n">
+        <f aca="false">B14/B13</f>
+        <v>4.62962962962963</v>
+      </c>
+      <c r="C15" s="7"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="0" t="n">
-        <v>200</v>
-      </c>
-      <c r="F15" s="0" t="n">
-        <v>350</v>
-      </c>
-      <c r="G15" s="1" t="n">
-        <v>400</v>
-      </c>
-      <c r="H15" s="1" t="n">
-        <v>700</v>
-      </c>
-      <c r="I15" s="0" t="n">
-        <v>400</v>
-      </c>
-      <c r="J15" s="0" t="n">
-        <v>350</v>
-      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="5" t="n">
-        <f aca="false">C14/B14</f>
-        <v>1.59341563786008</v>
+      <c r="B16" s="6" t="n">
+        <f aca="false">2.6/8</f>
+        <v>0.325</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="5" t="n">
-        <f aca="false">F15/E15</f>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="6" t="n">
+        <f aca="false">B6*B16</f>
+        <v>58.5</v>
+      </c>
+      <c r="C17" s="6" t="n">
+        <v>40</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1" t="n">
+        <f aca="false">180*0.4</f>
+        <v>72</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="6" t="n">
+        <f aca="false">B10*(1+B5/B6)</f>
+        <v>14.52</v>
+      </c>
+      <c r="C18" s="6" t="n">
+        <f aca="false">C10*(1+C5/C7)</f>
+        <v>13.5</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="0" t="n">
+        <v>17.5</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="8" t="n">
+        <f aca="false">B9*B10/(4*PI()*B8^2)</f>
+        <v>0.00036687926571624</v>
+      </c>
+      <c r="C19" s="8" t="n">
+        <f aca="false">C10*C9/(4*PI()*C5^2)</f>
+        <v>0.0015278874536822</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="9" t="n">
+        <f aca="false">B10*B9/(4*PI()*B8*B6)*(1-B16)</f>
+        <v>0.000665885867274975</v>
+      </c>
+      <c r="C20" s="9" t="n">
+        <f aca="false">C10*C9/(4*PI()*C8*C7)</f>
+        <v>0.00106103295394597</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" s="10" t="n">
+        <f aca="false">4*10^(-4)</f>
+        <v>0.0004</v>
+      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>350</v>
+      </c>
+      <c r="G22" s="12" t="n">
+        <v>400</v>
+      </c>
+      <c r="H22" s="1" t="n">
+        <v>650</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="J22" s="0" t="n">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="13" t="n">
+        <f aca="false">C20/B20</f>
+        <v>1.59341563786008</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="6" t="n">
+        <f aca="false">F22/E22</f>
         <v>1.75</v>
       </c>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5" t="n">
-        <f aca="false">H15/G15</f>
-        <v>1.75</v>
-      </c>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5" t="n">
-        <f aca="false">J15/I15</f>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6" t="n">
+        <f aca="false">H22/G22</f>
+        <v>1.625</v>
+      </c>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6" t="n">
+        <f aca="false">J22/I22</f>
         <v>0.875</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="0" t="n">
-        <f aca="false">C13/B13</f>
-        <v>0.929752066115703</v>
-      </c>
-      <c r="I17" s="0" t="n">
-        <f aca="false">J13/I13</f>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <f aca="false">C18/B18</f>
+        <v>0.929752066115702</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <f aca="false">J18/I18</f>
         <v>0.891428571428571</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="U18" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="V18" s="0" t="n">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="U25" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="V25" s="0" t="n">
         <f aca="false">4.4*10^(-2)*18/10</f>
         <v>0.0792</v>
       </c>
-      <c r="X18" s="0" t="n">
-        <f aca="false">EXP(-V18*5)</f>
+      <c r="X25" s="0" t="n">
+        <f aca="false">EXP(-V25*5)</f>
         <v>0.673006695937386</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="U19" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="V19" s="0" t="n">
-        <f aca="false">LN(2)/(V18*TAN(60*3.14159/180))</f>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="U26" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="V26" s="0" t="n">
+        <f aca="false">LN(2)/(V25*TAN(60*3.14159/180))</f>
         <v>5.05289809045416</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I21" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q21" s="8" t="s">
-        <v>26</v>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I28" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q28" s="15" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -957,8 +1277,8 @@
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A26:E26"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -986,9 +1306,9 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="3.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1000,96 +1320,96 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
-      <c r="B3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>5</v>
+      <c r="B3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="5" t="n">
+      <c r="A4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="6" t="n">
         <v>300</v>
       </c>
-      <c r="C4" s="5" t="n">
+      <c r="C4" s="6" t="n">
         <v>300</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="5" t="n">
+      <c r="A5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="6" t="n">
         <v>200</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="5" t="n">
+      <c r="A6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="6" t="n">
         <v>300</v>
       </c>
-      <c r="C6" s="5" t="n">
+      <c r="C6" s="6" t="n">
         <v>300</v>
       </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="5" t="n">
+      <c r="A7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="6" t="n">
         <f aca="false">B4+B5+B6</f>
         <v>800</v>
       </c>
-      <c r="C7" s="5" t="n">
+      <c r="C7" s="6" t="n">
         <f aca="false">SUM(C4:C6)</f>
         <v>600</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="5" t="n">
+      <c r="A8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="C8" s="5" t="n">
+      <c r="C8" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="D8" s="5"/>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="5" t="n">
+      <c r="A9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="6" t="n">
         <v>2</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="5" t="n">
+      <c r="A10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="6" t="n">
         <f aca="false">B9/(B8+B9)</f>
         <v>0.5</v>
       </c>
@@ -1097,59 +1417,59 @@
       <c r="D10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="5" t="n">
+      <c r="A11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="6" t="n">
         <f aca="false">B5*B10</f>
         <v>100</v>
       </c>
-      <c r="C11" s="5" t="n">
+      <c r="C11" s="6" t="n">
         <v>40</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="5" t="n">
+      <c r="A12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="6" t="n">
         <f aca="false">B8*(1+B4/B5)</f>
         <v>5</v>
       </c>
-      <c r="C12" s="5" t="n">
+      <c r="C12" s="6" t="n">
         <f aca="false">C8*(1+C4/C6)</f>
         <v>12</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="6" t="n">
+      <c r="A13" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="9" t="n">
         <f aca="false">B8*(1-B10)/(B7*B5)</f>
         <v>6.25E-006</v>
       </c>
-      <c r="C13" s="6" t="n">
+      <c r="C13" s="9" t="n">
         <f aca="false">C8/(C7*C6)</f>
         <v>3.33333333333333E-005</v>
       </c>
-      <c r="D13" s="5"/>
+      <c r="D13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
-        <v>18</v>
+      <c r="A14" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="5" t="n">
+      <c r="A15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="6" t="n">
         <f aca="false">C13/B13</f>
         <v>5.33333333333333</v>
       </c>
@@ -1157,20 +1477,20 @@
       <c r="D15" s="1"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
+      <c r="A17" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
+      <c r="A18" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1187,4 +1507,239 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G27"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.61"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="6" t="n">
+        <v>320</v>
+      </c>
+      <c r="C3" s="6" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="6" t="n">
+        <v>190</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="6" t="n">
+        <f aca="false">B3+B4+B5</f>
+        <v>510</v>
+      </c>
+      <c r="C6" s="6" t="n">
+        <f aca="false">SUM(C3:C5)</f>
+        <v>450</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="C8" s="6" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <f aca="false">B8+B9</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <f aca="false">B11/B10</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="6" t="n">
+        <f aca="false">B9/(B8+B9)</f>
+        <v>0.4</v>
+      </c>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="6" t="n">
+        <f aca="false">B4*B13</f>
+        <v>76</v>
+      </c>
+      <c r="C14" s="6" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="6" t="n">
+        <f aca="false">B8*(1+B3/B4)</f>
+        <v>8.05263157894737</v>
+      </c>
+      <c r="C15" s="6" t="n">
+        <f aca="false">C8*(1+C3/C5)</f>
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="9" t="n">
+        <f aca="false">B8*B7/(4*PI()*B6*B4)*(1-B13)</f>
+        <v>0.000147821928568324</v>
+      </c>
+      <c r="C16" s="9" t="n">
+        <f aca="false">C8*C7/(4*PI()*C6*C5)</f>
+        <v>0.00106103295394597</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="9" t="n">
+        <f aca="false">B12*B16</f>
+        <v>0.000739109642841619</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="6" t="n">
+        <f aca="false">C16/B17</f>
+        <v>1.43555555555556</v>
+      </c>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F26" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <f aca="false">4*10^(-4)</f>
+        <v>0.0004</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="0" t="n">
+        <f aca="false">100*3/(4*PI()*B6^2)</f>
+        <v>9.17848576077828E-005</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update of Introduction and MM section on the analytical model
</commit_message>
<xml_diff>
--- a/KES-MPS.xlsx
+++ b/KES-MPS.xlsx
@@ -5,12 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Brent" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Lin" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="AbsoluteEfficiency" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="KEStransparency" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="AllTogether" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="74">
   <si>
     <t xml:space="preserve">Simulation results</t>
   </si>
@@ -66,6 +68,9 @@
     <t xml:space="preserve">*</t>
   </si>
   <si>
+    <t xml:space="preserve">s_e (mm)</t>
+  </si>
+  <si>
     <t xml:space="preserve">septa (mm)</t>
   </si>
   <si>
@@ -139,19 +144,154 @@
   </si>
   <si>
     <t xml:space="preserve">Efficaicté KES publiée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://physics.nist.gov/cgi-bin/Xcom/xcom2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tungsten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Density</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy (MeV)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mu/rho (cm2/g)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mu (cm-1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">With of the knife-edge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Collimator thickness (mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Knife-edge angle (degree)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">With of the knife-edge (mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ln(2)/(mu*tan(alpha)) (mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lu2SiO5 (LSO)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thickness (cm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Detection efficiency (interaction prob.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CsI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smeets 2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lin 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Park 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Res (mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Published Res (mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Published eff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference for eff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AM eff / published eff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/(Estimated intrinsic absorber eff.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FOV factor</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Smeets 2016</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> – AM</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Lin 2017</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> – AM</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Park 2017 - AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Park 2017 – Published</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eff </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Park 2017 – AM corrected</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
     <numFmt numFmtId="166" formatCode="0.00E+000"/>
     <numFmt numFmtId="167" formatCode="#,##0.00"/>
+    <numFmt numFmtId="168" formatCode="0.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -180,8 +320,29 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -197,7 +358,19 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCCCCCC"/>
-        <bgColor rgb="FFCCCCFF"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFCCCCCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -242,7 +415,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -307,6 +480,70 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -341,7 +578,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -363,10 +600,10 @@
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFFF420E"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FFB3B3B3"/>
+      <rgbColor rgb="FF004586"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
@@ -377,6 +614,749 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Spatial resolution</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.168740168740169"/>
+          <c:y val="0.110895329150483"/>
+          <c:w val="0.715572715572716"/>
+          <c:h val="0.685489493078379"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>AllTogether!$B$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MPS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>AllTogether!$A$27:$A$29</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Smeets 2016 – AM</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Lin 2017 – AM</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Park 2017 - AM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>AllTogether!$B$27:$B$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>8.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>AllTogether!$C$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>KES</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>AllTogether!$A$27:$A$29</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Smeets 2016 – AM</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Lin 2017 – AM</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Park 2017 - AM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>AllTogether!$C$27:$C$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>23.6964791689616</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.063537039077</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.063537039077</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="1"/>
+        <c:axId val="86521968"/>
+        <c:axId val="37081438"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="86521968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="37081438"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="37081438"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Res (mm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="86521968"/>
+        <c:crossesAt val="1"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.562705562705563"/>
+          <c:y val="0.297480330644358"/>
+          <c:w val="0.170599170599171"/>
+          <c:h val="0.177372771636291"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Detection efficiency</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>AllTogether!$B$33</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MPS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>AllTogether!$A$34:$A$36</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Smeets 2016 – AM</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Lin 2017 – AM</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Park 2017 - AM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>AllTogether!$B$34:$B$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.00032740445436047</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.6314559621623E-005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.000568410511042483</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>AllTogether!$C$33</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>KES</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>AllTogether!$A$34:$A$36</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Smeets 2016 – AM</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Lin 2017 – AM</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Park 2017 - AM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>AllTogether!$C$34:$C$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.00120249585297877</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.000465606394273379</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.00209522877423021</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="1"/>
+        <c:axId val="74609025"/>
+        <c:axId val="97489750"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="74609025"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="97489750"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="97489750"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Eff</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="74609025"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.389430894308943"/>
+          <c:y val="0.242114615726344"/>
+          <c:w val="0.118824265165729"/>
+          <c:h val="0.121612616614838"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -390,9 +1370,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>464040</xdr:colOff>
+      <xdr:colOff>463320</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>51480</xdr:rowOff>
+      <xdr:rowOff>50760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -405,8 +1385,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9782280" y="0"/>
-          <a:ext cx="2032200" cy="2977560"/>
+          <a:off x="9781560" y="0"/>
+          <a:ext cx="2031480" cy="2976840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -427,9 +1407,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>352800</xdr:colOff>
+      <xdr:colOff>352080</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>19440</xdr:rowOff>
+      <xdr:rowOff>18720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -442,8 +1422,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7572240" y="56160"/>
-          <a:ext cx="2327040" cy="2889360"/>
+          <a:off x="7571520" y="56160"/>
+          <a:ext cx="2326320" cy="2888640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -464,9 +1444,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>282600</xdr:colOff>
+      <xdr:colOff>281880</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>61560</xdr:rowOff>
+      <xdr:rowOff>60840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -480,7 +1460,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="173880" y="4492080"/>
-          <a:ext cx="4000320" cy="4997880"/>
+          <a:ext cx="3999600" cy="4997160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -501,9 +1481,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>574200</xdr:colOff>
+      <xdr:colOff>573480</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>87120</xdr:rowOff>
+      <xdr:rowOff>86400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -516,8 +1496,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11965320" y="474480"/>
-          <a:ext cx="4168800" cy="1888200"/>
+          <a:off x="11964960" y="474480"/>
+          <a:ext cx="4167720" cy="1887480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -538,9 +1518,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>362880</xdr:colOff>
+      <xdr:colOff>362160</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>136440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -554,7 +1534,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4733640" y="4820400"/>
-          <a:ext cx="4574160" cy="3769560"/>
+          <a:ext cx="4573080" cy="3768840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -575,9 +1555,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>76320</xdr:colOff>
+      <xdr:colOff>75600</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>60840</xdr:rowOff>
+      <xdr:rowOff>60120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -590,8 +1570,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9943560" y="4930920"/>
-          <a:ext cx="4489920" cy="3745440"/>
+          <a:off x="9942840" y="4930920"/>
+          <a:ext cx="4489200" cy="3744720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -617,9 +1597,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>520920</xdr:colOff>
+      <xdr:colOff>520200</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>51480</xdr:rowOff>
+      <xdr:rowOff>50760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -633,7 +1613,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5666760" y="0"/>
-          <a:ext cx="2052360" cy="2977560"/>
+          <a:ext cx="2051640" cy="2976840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -654,9 +1634,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>233280</xdr:colOff>
+      <xdr:colOff>232560</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>126000</xdr:rowOff>
+      <xdr:rowOff>125280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -670,7 +1650,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3911760" y="0"/>
-          <a:ext cx="2316960" cy="2889360"/>
+          <a:ext cx="2316240" cy="2888640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -691,9 +1671,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>118080</xdr:colOff>
+      <xdr:colOff>117360</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>29520</xdr:rowOff>
+      <xdr:rowOff>28800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -707,7 +1687,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7958520" y="416880"/>
-          <a:ext cx="4168440" cy="1888200"/>
+          <a:ext cx="4167720" cy="1887480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -733,9 +1713,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>132840</xdr:colOff>
+      <xdr:colOff>132120</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>17280</xdr:rowOff>
+      <xdr:rowOff>16560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -749,7 +1729,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8138880" y="3657600"/>
-          <a:ext cx="4162320" cy="1886400"/>
+          <a:ext cx="4161600" cy="1885680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -770,9 +1750,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>300600</xdr:colOff>
+      <xdr:colOff>299880</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>155160</xdr:rowOff>
+      <xdr:rowOff>154440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -786,7 +1766,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14210280" y="30960"/>
-          <a:ext cx="2322720" cy="2887560"/>
+          <a:ext cx="2322000" cy="2886840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -801,15 +1781,80 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>553680</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>2160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>200520</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>40680</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="4835160" y="4228560"/>
+        <a:ext cx="5034960" cy="3614760"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>4320</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>87120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>71280</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>77400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="10707120" y="4313520"/>
+        <a:ext cx="5756400" cy="3241440"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:X28"/>
+  <dimension ref="A2:X29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="1" sqref="O4:O12 C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -987,9 +2032,15 @@
       <c r="A11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="B11" s="6" t="n">
+        <f aca="false">B10</f>
+        <v>5.4</v>
+      </c>
+      <c r="C11" s="6" t="n">
+        <f aca="false">C10+KEStransparency!B13</f>
+        <v>10.5317685195385</v>
+      </c>
+      <c r="D11" s="6"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="6"/>
@@ -1000,9 +2051,7 @@
         <v>15</v>
       </c>
       <c r="B12" s="6"/>
-      <c r="C12" s="1" t="n">
-        <v>4</v>
-      </c>
+      <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -1010,14 +2059,13 @@
       <c r="H12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="7" t="n">
-        <f aca="false">B10+B11</f>
-        <v>5.4</v>
-      </c>
-      <c r="C13" s="7"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="1" t="n">
+        <v>4</v>
+      </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -1029,7 +2077,8 @@
         <v>17</v>
       </c>
       <c r="B14" s="7" t="n">
-        <v>25</v>
+        <f aca="false">B10+B12</f>
+        <v>5.4</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="1"/>
@@ -1043,8 +2092,7 @@
         <v>18</v>
       </c>
       <c r="B15" s="7" t="n">
-        <f aca="false">B14/B13</f>
-        <v>4.62962962962963</v>
+        <v>25</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="1"/>
@@ -1054,14 +2102,14 @@
       <c r="H15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="6" t="n">
-        <f aca="false">2.6/8</f>
-        <v>0.325</v>
-      </c>
-      <c r="C16" s="1"/>
+      <c r="B16" s="7" t="n">
+        <f aca="false">B15/B14</f>
+        <v>4.62962962962963</v>
+      </c>
+      <c r="C16" s="7"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -1073,17 +2121,12 @@
         <v>20</v>
       </c>
       <c r="B17" s="6" t="n">
-        <f aca="false">B6*B16</f>
-        <v>58.5</v>
-      </c>
-      <c r="C17" s="6" t="n">
-        <v>40</v>
-      </c>
+        <f aca="false">2.6/8</f>
+        <v>0.325</v>
+      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="1" t="n">
-        <f aca="false">180*0.4</f>
-        <v>72</v>
-      </c>
+      <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
@@ -1093,56 +2136,58 @@
         <v>21</v>
       </c>
       <c r="B18" s="6" t="n">
-        <f aca="false">B10*(1+B5/B6)</f>
-        <v>14.52</v>
+        <f aca="false">B6*B17</f>
+        <v>58.5</v>
       </c>
       <c r="C18" s="6" t="n">
-        <f aca="false">C10*(1+C5/C7)</f>
-        <v>13.5</v>
+        <v>40</v>
       </c>
       <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="E18" s="1" t="n">
+        <f aca="false">180*0.4</f>
+        <v>72</v>
+      </c>
       <c r="F18" s="1"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
-      <c r="I18" s="0" t="n">
-        <v>17.5</v>
-      </c>
-      <c r="J18" s="0" t="n">
-        <v>15.6</v>
-      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="8" t="n">
-        <f aca="false">B9*B10/(4*PI()*B8^2)</f>
-        <v>0.00036687926571624</v>
-      </c>
-      <c r="C19" s="8" t="n">
-        <f aca="false">C10*C9/(4*PI()*C5^2)</f>
-        <v>0.0015278874536822</v>
+      <c r="B19" s="6" t="n">
+        <f aca="false">B10*(1+B5/B6)</f>
+        <v>14.52</v>
+      </c>
+      <c r="C19" s="6" t="n">
+        <f aca="false">C10*(1+C5/C7)</f>
+        <v>13.5</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
+      <c r="I19" s="0" t="n">
+        <v>17.5</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <v>15.6</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="9" t="n">
-        <f aca="false">B10*B9/(4*PI()*B8*B6)*(1-B16)</f>
-        <v>0.000665885867274975</v>
-      </c>
-      <c r="C20" s="9" t="n">
-        <f aca="false">C10*C9/(4*PI()*C8*C7)</f>
-        <v>0.00106103295394597</v>
-      </c>
-      <c r="D20" s="6"/>
+      <c r="B20" s="8" t="n">
+        <f aca="false">B9*B10/(4*PI()*B8^2)</f>
+        <v>0.00036687926571624</v>
+      </c>
+      <c r="C20" s="8" t="n">
+        <f aca="false">C10*C9/(4*PI()*C5^2)</f>
+        <v>0.0015278874536822</v>
+      </c>
+      <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="6"/>
@@ -1152,127 +2197,145 @@
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="10" t="n">
-        <f aca="false">4*10^(-4)</f>
-        <v>0.0004</v>
+      <c r="B21" s="9" t="n">
+        <f aca="false">B10*B9/(4*PI()*B8*B6)*(1-B17)</f>
+        <v>0.000665885867274975</v>
+      </c>
+      <c r="C21" s="9" t="n">
+        <f aca="false">C10*C9/(4*PI()*C8*C7)</f>
+        <v>0.00106103295394597</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
-      <c r="O21" s="0" t="n">
-        <f aca="false">SQRT(2)/B23</f>
-        <v>0.887535887543034</v>
-      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="0" t="n">
-        <v>200</v>
-      </c>
-      <c r="F22" s="0" t="n">
-        <v>350</v>
-      </c>
-      <c r="G22" s="12" t="n">
-        <v>400</v>
-      </c>
-      <c r="H22" s="1" t="n">
-        <v>650</v>
-      </c>
-      <c r="I22" s="0" t="n">
-        <v>400</v>
-      </c>
-      <c r="J22" s="0" t="n">
-        <v>350</v>
+      <c r="B22" s="9"/>
+      <c r="C22" s="10" t="n">
+        <f aca="false">4*10^(-4)</f>
+        <v>0.0004</v>
+      </c>
+      <c r="D22" s="6"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="O22" s="0" t="n">
+        <f aca="false">SQRT(2)/B24</f>
+        <v>0.887535887543033</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="13" t="n">
-        <f aca="false">C20/B20</f>
-        <v>1.59341563786008</v>
-      </c>
+      <c r="B23" s="6"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="6" t="n">
-        <f aca="false">F22/E22</f>
+      <c r="E23" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>350</v>
+      </c>
+      <c r="G23" s="12" t="n">
+        <v>400</v>
+      </c>
+      <c r="H23" s="1" t="n">
+        <v>650</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="J23" s="0" t="n">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="13" t="n">
+        <f aca="false">C21/B21</f>
+        <v>1.59341563786008</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="6" t="n">
+        <f aca="false">F23/E23</f>
         <v>1.75</v>
       </c>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6" t="n">
-        <f aca="false">H22/G22</f>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6" t="n">
+        <f aca="false">H23/G23</f>
         <v>1.625</v>
       </c>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6" t="n">
-        <f aca="false">J22/I22</f>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6" t="n">
+        <f aca="false">J23/I23</f>
         <v>0.875</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="0" t="n">
-        <f aca="false">C18/B18</f>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <f aca="false">C19/B19</f>
         <v>0.929752066115702</v>
       </c>
-      <c r="I24" s="0" t="n">
-        <f aca="false">J18/I18</f>
+      <c r="I25" s="0" t="n">
+        <f aca="false">J19/I19</f>
         <v>0.891428571428571</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="U25" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="V25" s="0" t="n">
-        <f aca="false">4.4*10^(-2)*18/10</f>
-        <v>0.0792</v>
-      </c>
-      <c r="X25" s="0" t="n">
-        <f aca="false">EXP(-V25*5)</f>
-        <v>0.673006695937386</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
       <c r="U26" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="V26" s="0" t="n">
+        <f aca="false">4.4*10^(-2)*18/10</f>
+        <v>0.0792</v>
+      </c>
+      <c r="X26" s="0" t="n">
+        <f aca="false">EXP(-V26*5)</f>
+        <v>0.673006695937386</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="V26" s="0" t="n">
-        <f aca="false">LN(2)/(V25*TAN(60*3.14159/180))</f>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="U27" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="V27" s="0" t="n">
+        <f aca="false">LN(2)/(V26*TAN(60*3.14159/180))</f>
         <v>5.05289809045416</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I28" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q28" s="15" t="s">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I29" s="15" t="s">
         <v>33</v>
+      </c>
+      <c r="Q29" s="15" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1281,8 +2344,8 @@
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
-    <mergeCell ref="A25:E25"/>
     <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A27:E27"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -1302,8 +2365,8 @@
   </sheetPr>
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C13" activeCellId="1" sqref="O4:O12 C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1324,7 +2387,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1"/>
@@ -1332,7 +2395,7 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>6</v>
@@ -1401,7 +2464,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="6" t="n">
         <v>2</v>
@@ -1411,7 +2474,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" s="6" t="n">
         <f aca="false">B9/(B8+B9)</f>
@@ -1422,7 +2485,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11" s="6" t="n">
         <f aca="false">B5*B10</f>
@@ -1435,7 +2498,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" s="6" t="n">
         <f aca="false">B8*(1+B4/B5)</f>
@@ -1449,21 +2512,21 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B13" s="9" t="n">
         <f aca="false">B8*(1-B10)/(B7*B5)</f>
         <v>6.25E-006</v>
       </c>
-      <c r="C13" s="9" t="n">
-        <f aca="false">C8/(C7*C6)</f>
-        <v>3.33333333333333E-005</v>
+      <c r="C13" s="9" t="e">
+        <f aca="false">C3*C2/(4*PI()*C1*#REF!)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1471,18 +2534,18 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="6" t="n">
+        <v>27</v>
+      </c>
+      <c r="B15" s="6" t="e">
         <f aca="false">C13/B13</f>
-        <v>5.33333333333333</v>
+        <v>#VALUE!</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
@@ -1490,7 +2553,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
@@ -1520,8 +2583,8 @@
   </sheetPr>
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A16" activeCellId="1" sqref="O4:O12 A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1614,7 +2677,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="6" t="n">
         <v>2</v>
@@ -1623,7 +2686,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" s="0" t="n">
         <f aca="false">B8+B9</f>
@@ -1632,7 +2695,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>25</v>
@@ -1640,7 +2703,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B12" s="0" t="n">
         <f aca="false">B11/B10</f>
@@ -1649,7 +2712,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B13" s="6" t="n">
         <f aca="false">B9/(B8+B9)</f>
@@ -1659,7 +2722,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" s="6" t="n">
         <f aca="false">B4*B13</f>
@@ -1671,7 +2734,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B15" s="6" t="n">
         <f aca="false">B8*(1+B3/B4)</f>
@@ -1684,7 +2747,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B16" s="9" t="n">
         <f aca="false">B8*B7/(4*PI()*B6*B4)*(1-B13)</f>
@@ -1697,7 +2760,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B17" s="9" t="n">
         <f aca="false">B12*B16</f>
@@ -1706,14 +2769,14 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B19" s="6" t="n">
         <f aca="false">C16/B17</f>
@@ -1723,7 +2786,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F26" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G26" s="0" t="n">
         <f aca="false">4*10^(-4)</f>
@@ -1746,4 +2809,1125 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F30"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B30" activeCellId="1" sqref="O4:O12 B30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.28"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="38.63"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1" s="16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="17" t="n">
+        <f aca="false">1.93*10</f>
+        <v>19.3</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="18" t="n">
+        <v>0.04038</v>
+      </c>
+      <c r="C5" s="18" t="n">
+        <f aca="false">B5*B3</f>
+        <v>0.779334</v>
+      </c>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <f aca="false">B8/2/TAN(B9*PI()/180)</f>
+        <v>10.1905089898886</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <f aca="false">LN(2)/(C5*TAN(B9*PI()/180))*10</f>
+        <v>4.5317685195385</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="B19" s="18" t="n">
+        <v>0.03785</v>
+      </c>
+      <c r="C19" s="18" t="n">
+        <f aca="false">B19*B17</f>
+        <v>0.28009</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <f aca="false">1-EXP(-C19*B21)</f>
+        <v>0.568406022677814</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>4.51</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="B27" s="18" t="n">
+        <v>0.0361</v>
+      </c>
+      <c r="C27" s="18" t="n">
+        <f aca="false">B27*B25</f>
+        <v>0.162811</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <f aca="false">1-EXP(-C27*B29)</f>
+        <v>0.386412867714185</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:P38"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O4" activeCellId="0" sqref="O4:O12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.89"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="1.29"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="5.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="1.29"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="10" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="3.12"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="20"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="N2" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="6"/>
+      <c r="J3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="6" t="n">
+        <v>250</v>
+      </c>
+      <c r="C4" s="6" t="n">
+        <v>220</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6" t="n">
+        <f aca="false">300-F5/2</f>
+        <v>200</v>
+      </c>
+      <c r="G4" s="6" t="n">
+        <v>300</v>
+      </c>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6" t="n">
+        <v>180</v>
+      </c>
+      <c r="K4" s="6" t="n">
+        <f aca="false">180+20</f>
+        <v>200</v>
+      </c>
+      <c r="L4" s="6"/>
+      <c r="N4" s="6" t="n">
+        <v>304</v>
+      </c>
+      <c r="O4" s="6" t="n">
+        <v>250</v>
+      </c>
+      <c r="P4" s="6"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="6" t="n">
+        <v>200</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="K5" s="1"/>
+      <c r="L5" s="6"/>
+      <c r="N5" s="6" t="n">
+        <v>180</v>
+      </c>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="6" t="n">
+        <v>176</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6" t="n">
+        <f aca="false">300-F5/2</f>
+        <v>200</v>
+      </c>
+      <c r="G6" s="6" t="n">
+        <v>300</v>
+      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="6" t="n">
+        <v>200</v>
+      </c>
+      <c r="L6" s="6"/>
+      <c r="N6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" s="6" t="n">
+        <v>200</v>
+      </c>
+      <c r="P6" s="6"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="6" t="n">
+        <f aca="false">B4+B5+B6</f>
+        <v>350</v>
+      </c>
+      <c r="C7" s="6" t="n">
+        <f aca="false">SUM(C4:C6)</f>
+        <v>396</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6" t="n">
+        <f aca="false">F4+F5+F6</f>
+        <v>600</v>
+      </c>
+      <c r="G7" s="6" t="n">
+        <f aca="false">SUM(G4:G6)</f>
+        <v>600</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6" t="n">
+        <f aca="false">J4+J5+J6</f>
+        <v>280</v>
+      </c>
+      <c r="K7" s="6" t="n">
+        <f aca="false">SUM(K4:K6)</f>
+        <v>400</v>
+      </c>
+      <c r="L7" s="6"/>
+      <c r="N7" s="6" t="n">
+        <f aca="false">N4+N5+N6</f>
+        <v>484</v>
+      </c>
+      <c r="O7" s="6" t="n">
+        <f aca="false">SUM(O4:O6)</f>
+        <v>450</v>
+      </c>
+      <c r="P7" s="6"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="K8" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="L8" s="6"/>
+      <c r="N8" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="O8" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="P8" s="1"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="6" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="C9" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="K9" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="L9" s="6"/>
+      <c r="N9" s="6" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="O9" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="P9" s="6"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="6" t="n">
+        <f aca="false">B9</f>
+        <v>2.4</v>
+      </c>
+      <c r="C10" s="6" t="n">
+        <f aca="false">C9+KEStransparency!$B13</f>
+        <v>10.5317685195385</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6" t="n">
+        <f aca="false">F9</f>
+        <v>2</v>
+      </c>
+      <c r="G10" s="6" t="n">
+        <f aca="false">G9+KEStransparency!$B13</f>
+        <v>10.5317685195385</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6" t="n">
+        <f aca="false">J9</f>
+        <v>2</v>
+      </c>
+      <c r="K10" s="6" t="n">
+        <f aca="false">K9+KEStransparency!$B13</f>
+        <v>10.5317685195385</v>
+      </c>
+      <c r="L10" s="6"/>
+      <c r="N10" s="6" t="n">
+        <f aca="false">N9</f>
+        <v>5.4</v>
+      </c>
+      <c r="O10" s="6" t="n">
+        <f aca="false">O9+KEStransparency!N12</f>
+        <v>6</v>
+      </c>
+      <c r="P10" s="6"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="6" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="K11" s="1"/>
+      <c r="L11" s="6"/>
+      <c r="N11" s="6" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="L12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="P12" s="1"/>
+    </row>
+    <row r="13" s="24" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="22" t="n">
+        <f aca="false">B9+B11</f>
+        <v>4</v>
+      </c>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22" t="n">
+        <f aca="false">F9+F11</f>
+        <v>4</v>
+      </c>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22" t="n">
+        <f aca="false">J9+J11</f>
+        <v>4</v>
+      </c>
+      <c r="K13" s="22" t="n">
+        <v>4</v>
+      </c>
+      <c r="L13" s="23"/>
+      <c r="N13" s="22" t="n">
+        <f aca="false">N9+N11</f>
+        <v>8</v>
+      </c>
+      <c r="O13" s="22"/>
+      <c r="P13" s="22"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="6" t="n">
+        <f aca="false">B11/B13</f>
+        <v>0.4</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="6" t="n">
+        <f aca="false">F11/F13</f>
+        <v>0.5</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="6" t="n">
+        <f aca="false">J11/J13</f>
+        <v>0.5</v>
+      </c>
+      <c r="K14" s="1"/>
+      <c r="L14" s="6"/>
+      <c r="N14" s="6" t="n">
+        <f aca="false">N11/N13</f>
+        <v>0.325</v>
+      </c>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="6" t="n">
+        <f aca="false">B5*B14</f>
+        <v>40</v>
+      </c>
+      <c r="C15" s="6" t="n">
+        <v>40</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6" t="n">
+        <f aca="false">F5*F14</f>
+        <v>100</v>
+      </c>
+      <c r="G15" s="6" t="n">
+        <v>40</v>
+      </c>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6" t="n">
+        <f aca="false">J5*J14</f>
+        <v>50</v>
+      </c>
+      <c r="K15" s="6" t="n">
+        <v>40</v>
+      </c>
+      <c r="L15" s="6"/>
+      <c r="N15" s="6" t="n">
+        <f aca="false">N5*N14</f>
+        <v>58.5</v>
+      </c>
+      <c r="O15" s="6" t="n">
+        <v>40</v>
+      </c>
+      <c r="P15" s="6"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="26" t="n">
+        <f aca="false">B10*(1+B4/B5)</f>
+        <v>8.4</v>
+      </c>
+      <c r="C16" s="26" t="n">
+        <f aca="false">C10*(1+C4/C6)</f>
+        <v>23.6964791689616</v>
+      </c>
+      <c r="D16" s="27" t="n">
+        <f aca="false">C16/B16</f>
+        <v>2.82100942487638</v>
+      </c>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26" t="n">
+        <f aca="false">F10*(1+F4/F5)</f>
+        <v>4</v>
+      </c>
+      <c r="G16" s="26" t="n">
+        <f aca="false">G10*(1+G4/G6)</f>
+        <v>21.063537039077</v>
+      </c>
+      <c r="H16" s="27" t="n">
+        <f aca="false">G16/F16</f>
+        <v>5.26588425976925</v>
+      </c>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26" t="n">
+        <f aca="false">J10*(1+J4/J5)</f>
+        <v>5.6</v>
+      </c>
+      <c r="K16" s="26" t="n">
+        <f aca="false">K10*(1+K4/K6)</f>
+        <v>21.063537039077</v>
+      </c>
+      <c r="L16" s="27" t="n">
+        <f aca="false">K16/J16</f>
+        <v>3.76134589983518</v>
+      </c>
+      <c r="N16" s="26" t="n">
+        <f aca="false">N10*(1+N4/N5)</f>
+        <v>14.52</v>
+      </c>
+      <c r="O16" s="26" t="n">
+        <f aca="false">O10*(1+O4/O6)</f>
+        <v>13.5</v>
+      </c>
+      <c r="P16" s="27" t="n">
+        <f aca="false">O16/N16</f>
+        <v>0.929752066115702</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="K17" s="26" t="n">
+        <v>20.6</v>
+      </c>
+      <c r="L17" s="27" t="n">
+        <f aca="false">K17/J17</f>
+        <v>3.26984126984127</v>
+      </c>
+      <c r="N17" s="26"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="27"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="28" t="n">
+        <f aca="false">B8*B10/(4*PI()*B7*B5)*(1-B14)</f>
+        <v>0.00032740445436047</v>
+      </c>
+      <c r="C18" s="28" t="n">
+        <f aca="false">C8*C10/(4*PI()*C7*C6)</f>
+        <v>0.00120249585297877</v>
+      </c>
+      <c r="D18" s="27" t="n">
+        <f aca="false">C18/B18</f>
+        <v>3.67281457831001</v>
+      </c>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28" t="n">
+        <f aca="false">F8*F10/(4*PI()*F7*F5)*(1-F14)</f>
+        <v>6.6314559621623E-005</v>
+      </c>
+      <c r="G18" s="28" t="n">
+        <f aca="false">G8*G10/(4*PI()*G7*G6)</f>
+        <v>0.000465606394273379</v>
+      </c>
+      <c r="H18" s="27" t="n">
+        <f aca="false">G18/F18</f>
+        <v>7.02117901302567</v>
+      </c>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28" t="n">
+        <f aca="false">J8*J10/(4*PI()*J7*J5)*(1-J14)</f>
+        <v>0.000568410511042483</v>
+      </c>
+      <c r="K18" s="28" t="n">
+        <f aca="false">K8*K10/(4*PI()*K7*K6)</f>
+        <v>0.00209522877423021</v>
+      </c>
+      <c r="L18" s="27" t="n">
+        <f aca="false">K18/J18</f>
+        <v>3.68611898183848</v>
+      </c>
+      <c r="N18" s="28" t="n">
+        <f aca="false">N8*N10/(4*PI()*N7*N5)*(1-N14)</f>
+        <v>0.000665885867274975</v>
+      </c>
+      <c r="O18" s="28" t="n">
+        <f aca="false">O8*O10/(4*PI()*O7*O6)</f>
+        <v>0.00106103295394597</v>
+      </c>
+      <c r="P18" s="27" t="n">
+        <f aca="false">O18/N18</f>
+        <v>1.59341563786008</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="9"/>
+      <c r="C19" s="29" t="n">
+        <f aca="false">4*10^(-4)</f>
+        <v>0.0004</v>
+      </c>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="9" t="n">
+        <f aca="false">3*10^(-4)</f>
+        <v>0.0003</v>
+      </c>
+      <c r="K19" s="29" t="n">
+        <f aca="false">7.2*10^(-4)</f>
+        <v>0.00072</v>
+      </c>
+      <c r="L19" s="27" t="n">
+        <f aca="false">K19/J19</f>
+        <v>2.4</v>
+      </c>
+      <c r="N19" s="9"/>
+      <c r="O19" s="29" t="n">
+        <f aca="false">4*10^(-4)</f>
+        <v>0.0004</v>
+      </c>
+      <c r="P19" s="29"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="K20" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="J21" s="0" t="n">
+        <f aca="false">J18/J19</f>
+        <v>1.89470170347494</v>
+      </c>
+      <c r="K21" s="0" t="n">
+        <f aca="false">K18/K19</f>
+        <v>2.91003996420862</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="J22" s="0" t="n">
+        <f aca="false">1/KEStransparency!B30</f>
+        <v>2.58790553719257</v>
+      </c>
+      <c r="K22" s="0" t="n">
+        <f aca="false">1/KEStransparency!B22</f>
+        <v>1.75930577809311</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="J23" s="0" t="n">
+        <f aca="false">J16/J13</f>
+        <v>1.4</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <f aca="false">K16/K13</f>
+        <v>5.26588425976925</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="31" t="n">
+        <f aca="false">B16</f>
+        <v>8.4</v>
+      </c>
+      <c r="C27" s="31" t="n">
+        <f aca="false">C16</f>
+        <v>23.6964791689616</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="31" t="n">
+        <f aca="false">F16</f>
+        <v>4</v>
+      </c>
+      <c r="C28" s="31" t="n">
+        <f aca="false">G16</f>
+        <v>21.063537039077</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="31" t="n">
+        <f aca="false">J16</f>
+        <v>5.6</v>
+      </c>
+      <c r="C29" s="31" t="n">
+        <f aca="false">K16</f>
+        <v>21.063537039077</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="31" t="n">
+        <f aca="false">J17</f>
+        <v>6.3</v>
+      </c>
+      <c r="C30" s="31" t="n">
+        <f aca="false">K17</f>
+        <v>20.6</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34" s="31" t="n">
+        <f aca="false">B18</f>
+        <v>0.00032740445436047</v>
+      </c>
+      <c r="C34" s="31" t="n">
+        <f aca="false">C18</f>
+        <v>0.00120249585297877</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" s="31" t="n">
+        <f aca="false">F18</f>
+        <v>6.6314559621623E-005</v>
+      </c>
+      <c r="C35" s="31" t="n">
+        <f aca="false">G18</f>
+        <v>0.000465606394273379</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="31" t="n">
+        <f aca="false">J18</f>
+        <v>0.000568410511042483</v>
+      </c>
+      <c r="C36" s="31" t="n">
+        <f aca="false">K18</f>
+        <v>0.00209522877423021</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="31" t="n">
+        <f aca="false">B36*KEStransparency!B30</f>
+        <v>0.000219641135610811</v>
+      </c>
+      <c r="C37" s="31" t="n">
+        <f aca="false">C36*KEStransparency!B22</f>
+        <v>0.0011909406541603</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" s="31" t="n">
+        <f aca="false">J19</f>
+        <v>0.0003</v>
+      </c>
+      <c r="C38" s="31" t="n">
+        <f aca="false">K19</f>
+        <v>0.00072</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="N2:P2"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Finalization of MM section review + update of the table for AMV
</commit_message>
<xml_diff>
--- a/KES-MPS.xlsx
+++ b/KES-MPS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Brent" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="81">
   <si>
     <t xml:space="preserve">Simulation results</t>
   </si>
@@ -146,7 +146,7 @@
     <t xml:space="preserve">Efficaicté KES publiée</t>
   </si>
   <si>
-    <t xml:space="preserve">https://physics.nist.gov/cgi-bin/Xcom/xcom2</t>
+    <t xml:space="preserve">https://www.physics.nist.gov/PhysRefData/Xcom/html/xcom1.html</t>
   </si>
   <si>
     <t xml:space="preserve">Tungsten</t>
@@ -191,6 +191,12 @@
     <t xml:space="preserve">CsI</t>
   </si>
   <si>
+    <t xml:space="preserve">BGO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brent</t>
+  </si>
+  <si>
     <t xml:space="preserve">Smeets 2016</t>
   </si>
   <si>
@@ -200,72 +206,55 @@
     <t xml:space="preserve">Park 2017</t>
   </si>
   <si>
-    <t xml:space="preserve">Brent</t>
+    <t xml:space="preserve">Analytical model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MC simulations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ecarts relatifs</t>
   </si>
   <si>
     <t xml:space="preserve">Ratio</t>
   </si>
   <si>
+    <t xml:space="preserve">Res (mm) Physical collimator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Res (mm) Perfect collimator </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Published Res (mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eff Physical collimator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eff Perfect collimator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Published eff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference for eff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AM eff / published eff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/(Estimated intrinsic absorber eff.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FOV factor</t>
+  </si>
+  <si>
     <t xml:space="preserve">Res (mm)</t>
   </si>
   <si>
-    <t xml:space="preserve">Published Res (mm)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Published eff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference for eff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AM eff / published eff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1/(Estimated intrinsic absorber eff.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FOV factor</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Smeets 2016</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> – AM</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Lin 2017</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> – AM</t>
-    </r>
+    <t xml:space="preserve">Smeets 2016 – AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lin 2017 – AM</t>
   </si>
   <si>
     <t xml:space="preserve">Park 2017 - AM</t>
@@ -291,7 +280,7 @@
     <numFmt numFmtId="167" formatCode="#,##0.00"/>
     <numFmt numFmtId="168" formatCode="0.00"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -322,17 +311,24 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="13"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -342,7 +338,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -369,8 +365,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFE0EFD4"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBCE4E5"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFE0EFD4"/>
       </patternFill>
     </fill>
   </fills>
@@ -415,7 +423,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="40">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -480,11 +488,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -504,7 +516,43 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -512,31 +560,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -574,7 +614,7 @@
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFBCE4E5"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
@@ -589,7 +629,7 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFE0EFD4"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
@@ -616,7 +656,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -656,10 +696,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.168740168740169"/>
-          <c:y val="0.110895329150483"/>
-          <c:w val="0.715572715572716"/>
-          <c:h val="0.685489493078379"/>
+          <c:x val="0.168752234537004"/>
+          <c:y val="0.110856573705179"/>
+          <c:w val="0.715480872363246"/>
+          <c:h val="0.685358565737052"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -670,7 +710,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>AllTogether!$B$26</c:f>
+              <c:f>AllTogether!$B$28:$B$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -701,6 +741,7 @@
           </c:marker>
           <c:dLbls>
             <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -710,7 +751,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>AllTogether!$A$27:$A$29</c:f>
+              <c:f>AllTogether!$A$29:$A$31</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -727,7 +768,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>AllTogether!$B$27:$B$29</c:f>
+              <c:f>AllTogether!$B$29:$B$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -750,7 +791,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>AllTogether!$C$26</c:f>
+              <c:f>AllTogether!$C$28:$C$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -781,6 +822,7 @@
           </c:marker>
           <c:dLbls>
             <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -790,7 +832,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>AllTogether!$A$27:$A$29</c:f>
+              <c:f>AllTogether!$A$29:$A$31</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -807,7 +849,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>AllTogether!$C$27:$C$29</c:f>
+              <c:f>AllTogether!$C$29:$C$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -833,11 +875,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="86521968"/>
-        <c:axId val="37081438"/>
+        <c:axId val="84877201"/>
+        <c:axId val="26537259"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="86521968"/>
+        <c:axId val="84877201"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -865,14 +907,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37081438"/>
+        <c:crossAx val="26537259"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="37081438"/>
+        <c:axId val="26537259"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -937,7 +979,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86521968"/>
+        <c:crossAx val="84877201"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -993,7 +1035,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1036,7 +1078,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>AllTogether!$B$33</c:f>
+              <c:f>AllTogether!$B$35:$B$35</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1067,6 +1109,7 @@
           </c:marker>
           <c:dLbls>
             <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1076,7 +1119,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>AllTogether!$A$34:$A$36</c:f>
+              <c:f>AllTogether!$A$36:$A$38</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1093,7 +1136,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>AllTogether!$B$34:$B$36</c:f>
+              <c:f>AllTogether!$B$36:$B$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1116,7 +1159,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>AllTogether!$C$33</c:f>
+              <c:f>AllTogether!$C$35:$C$35</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1147,6 +1190,7 @@
           </c:marker>
           <c:dLbls>
             <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1156,7 +1200,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>AllTogether!$A$34:$A$36</c:f>
+              <c:f>AllTogether!$A$36:$A$38</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1173,7 +1217,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>AllTogether!$C$34:$C$36</c:f>
+              <c:f>AllTogether!$C$36:$C$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1199,11 +1243,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="74609025"/>
-        <c:axId val="97489750"/>
+        <c:axId val="8445730"/>
+        <c:axId val="83949643"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="74609025"/>
+        <c:axId val="8445730"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1231,14 +1275,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97489750"/>
+        <c:crossAx val="83949643"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97489750"/>
+        <c:axId val="83949643"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1281,7 +1325,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1303,7 +1347,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74609025"/>
+        <c:crossAx val="8445730"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1370,9 +1414,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>463320</xdr:colOff>
+      <xdr:colOff>462600</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>50760</xdr:rowOff>
+      <xdr:rowOff>50040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1386,7 +1430,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9781560" y="0"/>
-          <a:ext cx="2031480" cy="2976840"/>
+          <a:ext cx="2030760" cy="2976120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1407,9 +1451,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>352080</xdr:colOff>
+      <xdr:colOff>351360</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>18720</xdr:rowOff>
+      <xdr:rowOff>18000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1423,7 +1467,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7571520" y="56160"/>
-          <a:ext cx="2326320" cy="2888640"/>
+          <a:ext cx="2325600" cy="2887920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1444,9 +1488,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>281880</xdr:colOff>
+      <xdr:colOff>281160</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>60840</xdr:rowOff>
+      <xdr:rowOff>60120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1460,7 +1504,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="173880" y="4492080"/>
-          <a:ext cx="3999600" cy="4997160"/>
+          <a:ext cx="3998880" cy="4996440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1481,9 +1525,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>573480</xdr:colOff>
+      <xdr:colOff>572760</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>86400</xdr:rowOff>
+      <xdr:rowOff>85680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1497,7 +1541,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11964960" y="474480"/>
-          <a:ext cx="4167720" cy="1887480"/>
+          <a:ext cx="4167000" cy="1886760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1518,9 +1562,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>362160</xdr:colOff>
+      <xdr:colOff>361440</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>136440</xdr:rowOff>
+      <xdr:rowOff>135720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1534,7 +1578,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4733640" y="4820400"/>
-          <a:ext cx="4573080" cy="3768840"/>
+          <a:ext cx="4572360" cy="3768120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1555,9 +1599,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>75600</xdr:colOff>
+      <xdr:colOff>74880</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>60120</xdr:rowOff>
+      <xdr:rowOff>59400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1571,7 +1615,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9942840" y="4930920"/>
-          <a:ext cx="4489200" cy="3744720"/>
+          <a:ext cx="4488480" cy="3744000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1597,9 +1641,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>520200</xdr:colOff>
+      <xdr:colOff>519480</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>50760</xdr:rowOff>
+      <xdr:rowOff>50040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1613,7 +1657,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5666760" y="0"/>
-          <a:ext cx="2051640" cy="2976840"/>
+          <a:ext cx="2050920" cy="2976120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1634,9 +1678,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>232560</xdr:colOff>
+      <xdr:colOff>231840</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>125280</xdr:rowOff>
+      <xdr:rowOff>124560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1650,7 +1694,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3911760" y="0"/>
-          <a:ext cx="2316240" cy="2888640"/>
+          <a:ext cx="2315520" cy="2887920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1671,9 +1715,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>117360</xdr:colOff>
+      <xdr:colOff>116640</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>28800</xdr:rowOff>
+      <xdr:rowOff>28080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1687,7 +1731,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7958520" y="416880"/>
-          <a:ext cx="4167720" cy="1887480"/>
+          <a:ext cx="4167000" cy="1886760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1713,9 +1757,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>132120</xdr:colOff>
+      <xdr:colOff>131400</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>16560</xdr:rowOff>
+      <xdr:rowOff>15840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1729,7 +1773,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8138880" y="3657600"/>
-          <a:ext cx="4161600" cy="1885680"/>
+          <a:ext cx="4160880" cy="1884960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1750,9 +1794,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>299880</xdr:colOff>
+      <xdr:colOff>299160</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>154440</xdr:rowOff>
+      <xdr:rowOff>153720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1766,7 +1810,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14210280" y="30960"/>
-          <a:ext cx="2322000" cy="2886840"/>
+          <a:ext cx="2321280" cy="2886120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1786,15 +1830,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>553680</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>2160</xdr:rowOff>
+      <xdr:colOff>554040</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>2520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>200520</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>40680</xdr:rowOff>
+      <xdr:colOff>200160</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>40320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1802,8 +1846,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4835160" y="4228560"/>
-        <a:ext cx="5034960" cy="3614760"/>
+        <a:off x="4835520" y="4554000"/>
+        <a:ext cx="5034240" cy="3614040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1817,14 +1861,14 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>4320</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>87120</xdr:rowOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>87480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>71280</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>77400</xdr:rowOff>
+      <xdr:colOff>70920</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>77040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1832,8 +1876,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10707120" y="4313520"/>
-        <a:ext cx="5756400" cy="3241440"/>
+        <a:off x="10707120" y="4638960"/>
+        <a:ext cx="5756040" cy="3240720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1854,7 +1898,7 @@
   <dimension ref="A2:X29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="1" sqref="O4:O12 C5"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2366,7 +2410,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="1" sqref="O4:O12 C13"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2584,7 +2628,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="1" sqref="O4:O12 A16"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2816,10 +2860,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="1" sqref="O4:O12 B30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2831,13 +2875,13 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F1" s="16" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="17" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2845,43 +2889,43 @@
       <c r="A3" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="17" t="n">
+      <c r="B3" s="18" t="n">
         <f aca="false">1.93*10</f>
         <v>19.3</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="18" t="n">
+      <c r="A5" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="18" t="n">
+      <c r="B5" s="19" t="n">
         <v>0.04038</v>
       </c>
-      <c r="C5" s="18" t="n">
+      <c r="C5" s="19" t="n">
         <f aca="false">B5*B3</f>
         <v>0.779334</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -2905,7 +2949,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="19" t="s">
         <v>49</v>
       </c>
       <c r="B10" s="0" t="n">
@@ -2923,7 +2967,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="20" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2936,24 +2980,24 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="19" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="18" t="n">
+      <c r="A19" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="B19" s="18" t="n">
+      <c r="B19" s="19" t="n">
         <v>0.03785</v>
       </c>
-      <c r="C19" s="18" t="n">
+      <c r="C19" s="19" t="n">
         <f aca="false">B19*B17</f>
         <v>0.28009</v>
       </c>
@@ -2976,7 +3020,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="20" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2989,24 +3033,24 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="18" t="s">
+      <c r="A26" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="19" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="18" t="n">
+      <c r="A27" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="B27" s="18" t="n">
+      <c r="B27" s="19" t="n">
         <v>0.0361</v>
       </c>
-      <c r="C27" s="18" t="n">
+      <c r="C27" s="19" t="n">
         <f aca="false">B27*B25</f>
         <v>0.162811</v>
       </c>
@@ -3028,7 +3072,63 @@
         <v>0.386412867714185</v>
       </c>
     </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>7.13</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="19" t="n">
+        <v>4</v>
+      </c>
+      <c r="B35" s="19" t="n">
+        <v>0.0389</v>
+      </c>
+      <c r="C35" s="19" t="n">
+        <f aca="false">B35*B33</f>
+        <v>0.277357</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <f aca="false">1-EXP(-C35*B37)</f>
+        <v>0.564852837279011</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F1" r:id="rId1" display="https://www.physics.nist.gov/PhysRefData/Xcom/html/xcom1.html"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3044,10 +3144,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P38"/>
+  <dimension ref="A1:T40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O4" activeCellId="0" sqref="O4:O12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T20" activeCellId="0" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3066,36 +3166,53 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="20"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
+      <c r="A1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="N1" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
-      <c r="B2" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
+      <c r="B2" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="F2" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="N2" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
+      <c r="J2" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="N2" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="R2" s="3"/>
+      <c r="S2" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="T2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
@@ -3106,7 +3223,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="1" t="s">
@@ -3116,7 +3233,7 @@
         <v>6</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="1" t="s">
@@ -3126,7 +3243,7 @@
         <v>6</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>5</v>
@@ -3135,7 +3252,19 @@
         <v>6</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>59</v>
+        <v>63</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3174,6 +3303,10 @@
         <v>250</v>
       </c>
       <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
@@ -3201,6 +3334,10 @@
       </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
@@ -3237,6 +3374,10 @@
         <v>200</v>
       </c>
       <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
@@ -3280,6 +3421,10 @@
         <v>450</v>
       </c>
       <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
@@ -3315,6 +3460,10 @@
         <v>200</v>
       </c>
       <c r="P8" s="1"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
@@ -3350,6 +3499,10 @@
         <v>6</v>
       </c>
       <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
@@ -3389,10 +3542,14 @@
         <v>5.4</v>
       </c>
       <c r="O10" s="6" t="n">
-        <f aca="false">O9+KEStransparency!N12</f>
-        <v>6</v>
+        <f aca="false">O9+KEStransparency!$B13</f>
+        <v>10.5317685195385</v>
       </c>
       <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
@@ -3420,6 +3577,10 @@
       </c>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
@@ -3447,39 +3608,47 @@
         <v>4</v>
       </c>
       <c r="P12" s="1"/>
-    </row>
-    <row r="13" s="24" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="22" t="s">
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="22" t="n">
+      <c r="B13" s="6" t="n">
         <f aca="false">B9+B11</f>
         <v>4</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22" t="n">
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6" t="n">
         <f aca="false">F9+F11</f>
         <v>4</v>
       </c>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22" t="n">
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6" t="n">
         <f aca="false">J9+J11</f>
         <v>4</v>
       </c>
-      <c r="K13" s="22" t="n">
+      <c r="K13" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="L13" s="23"/>
-      <c r="N13" s="22" t="n">
+      <c r="L13" s="1"/>
+      <c r="N13" s="6" t="n">
         <f aca="false">N9+N11</f>
         <v>8</v>
       </c>
-      <c r="O13" s="22"/>
-      <c r="P13" s="22"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
@@ -3511,6 +3680,10 @@
       </c>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
@@ -3550,376 +3723,491 @@
         <v>40</v>
       </c>
       <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" s="26" t="n">
+      <c r="A16" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="25" t="n">
         <f aca="false">B10*(1+B4/B5)</f>
         <v>8.4</v>
       </c>
-      <c r="C16" s="26" t="n">
-        <f aca="false">C10*(1+C4/C6)</f>
+      <c r="C16" s="25" t="n">
+        <f aca="false">C10*(1+C$4/C$6)</f>
         <v>23.6964791689616</v>
       </c>
-      <c r="D16" s="27" t="n">
+      <c r="D16" s="25" t="n">
         <f aca="false">C16/B16</f>
         <v>2.82100942487638</v>
       </c>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26" t="n">
+      <c r="E16" s="25"/>
+      <c r="F16" s="25" t="n">
         <f aca="false">F10*(1+F4/F5)</f>
         <v>4</v>
       </c>
-      <c r="G16" s="26" t="n">
-        <f aca="false">G10*(1+G4/G6)</f>
+      <c r="G16" s="25" t="n">
+        <f aca="false">G10*(1+G$4/G$6)</f>
         <v>21.063537039077</v>
       </c>
-      <c r="H16" s="27" t="n">
+      <c r="H16" s="25" t="n">
         <f aca="false">G16/F16</f>
         <v>5.26588425976925</v>
       </c>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26" t="n">
+      <c r="I16" s="25"/>
+      <c r="J16" s="25" t="n">
         <f aca="false">J10*(1+J4/J5)</f>
         <v>5.6</v>
       </c>
-      <c r="K16" s="26" t="n">
-        <f aca="false">K10*(1+K4/K6)</f>
+      <c r="K16" s="25" t="n">
+        <f aca="false">K10*(1+K$4/K$6)</f>
         <v>21.063537039077</v>
       </c>
-      <c r="L16" s="27" t="n">
+      <c r="L16" s="25" t="n">
         <f aca="false">K16/J16</f>
         <v>3.76134589983518</v>
       </c>
-      <c r="N16" s="26" t="n">
+      <c r="M16" s="26"/>
+      <c r="N16" s="25" t="n">
         <f aca="false">N10*(1+N4/N5)</f>
         <v>14.52</v>
       </c>
-      <c r="O16" s="26" t="n">
-        <f aca="false">O10*(1+O4/O6)</f>
+      <c r="O16" s="25" t="n">
+        <f aca="false">O10*(1+O$4/O$6)</f>
+        <v>23.6964791689616</v>
+      </c>
+      <c r="P16" s="25" t="n">
+        <f aca="false">O16/N16</f>
+        <v>1.63198892348221</v>
+      </c>
+      <c r="Q16" s="27" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="R16" s="27" t="n">
+        <v>19.3</v>
+      </c>
+      <c r="S16" s="27" t="n">
+        <f aca="false">(Q16-N16)/Q16</f>
+        <v>0.354666666666667</v>
+      </c>
+      <c r="T16" s="27" t="n">
+        <f aca="false">(R16-O16)/R16</f>
+        <v>-0.227796848132727</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="24"/>
+      <c r="C17" s="25" t="n">
+        <f aca="false">C9*(1+C$4/C$6)</f>
         <v>13.5</v>
       </c>
-      <c r="P16" s="27" t="n">
-        <f aca="false">O16/N16</f>
-        <v>0.929752066115702</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26" t="n">
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="25" t="n">
+        <f aca="false">G9*(1+G$4/G$6)</f>
+        <v>12</v>
+      </c>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="25" t="n">
+        <f aca="false">K9*(1+K$4/K$6)</f>
+        <v>12</v>
+      </c>
+      <c r="L17" s="24"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="25" t="n">
+        <f aca="false">O9*(1+O$4/O$6)</f>
+        <v>13.5</v>
+      </c>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="27"/>
+      <c r="R17" s="27" t="n">
+        <v>12</v>
+      </c>
+      <c r="S17" s="27"/>
+      <c r="T17" s="27" t="n">
+        <f aca="false">(R17-O17)/R17</f>
+        <v>-0.125</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30" t="n">
         <v>6.3</v>
       </c>
-      <c r="K17" s="26" t="n">
+      <c r="K18" s="30" t="n">
         <v>20.6</v>
       </c>
-      <c r="L17" s="27" t="n">
-        <f aca="false">K17/J17</f>
+      <c r="L18" s="31" t="n">
+        <f aca="false">K18/J18</f>
         <v>3.26984126984127</v>
       </c>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
-      <c r="P17" s="27"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="B18" s="28" t="n">
+      <c r="M18" s="32"/>
+      <c r="Q18" s="33"/>
+      <c r="R18" s="33"/>
+      <c r="S18" s="33"/>
+      <c r="T18" s="33"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="35" t="n">
         <f aca="false">B8*B10/(4*PI()*B7*B5)*(1-B14)</f>
         <v>0.00032740445436047</v>
       </c>
-      <c r="C18" s="28" t="n">
+      <c r="C19" s="35" t="n">
         <f aca="false">C8*C10/(4*PI()*C7*C6)</f>
         <v>0.00120249585297877</v>
       </c>
-      <c r="D18" s="27" t="n">
-        <f aca="false">C18/B18</f>
-        <v>3.67281457831001</v>
-      </c>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28" t="n">
+      <c r="D19" s="36" t="n">
+        <f aca="false">C19/B19</f>
+        <v>3.67281457831</v>
+      </c>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35" t="n">
         <f aca="false">F8*F10/(4*PI()*F7*F5)*(1-F14)</f>
         <v>6.6314559621623E-005</v>
       </c>
-      <c r="G18" s="28" t="n">
+      <c r="G19" s="35" t="n">
         <f aca="false">G8*G10/(4*PI()*G7*G6)</f>
         <v>0.000465606394273379</v>
       </c>
-      <c r="H18" s="27" t="n">
-        <f aca="false">G18/F18</f>
+      <c r="H19" s="36" t="n">
+        <f aca="false">G19/F19</f>
         <v>7.02117901302567</v>
       </c>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28" t="n">
+      <c r="I19" s="35"/>
+      <c r="J19" s="35" t="n">
         <f aca="false">J8*J10/(4*PI()*J7*J5)*(1-J14)</f>
         <v>0.000568410511042483</v>
       </c>
-      <c r="K18" s="28" t="n">
+      <c r="K19" s="35" t="n">
         <f aca="false">K8*K10/(4*PI()*K7*K6)</f>
         <v>0.00209522877423021</v>
       </c>
-      <c r="L18" s="27" t="n">
-        <f aca="false">K18/J18</f>
-        <v>3.68611898183848</v>
-      </c>
-      <c r="N18" s="28" t="n">
-        <f aca="false">N8*N10/(4*PI()*N7*N5)*(1-N14)</f>
+      <c r="L19" s="36" t="n">
+        <f aca="false">K19/J19</f>
+        <v>3.68611898183847</v>
+      </c>
+      <c r="M19" s="37"/>
+      <c r="N19" s="35"/>
+      <c r="O19" s="35"/>
+      <c r="P19" s="36"/>
+      <c r="Q19" s="35" t="n">
+        <f aca="false">3.4*10^(-4)</f>
+        <v>0.00034</v>
+      </c>
+      <c r="R19" s="35" t="n">
+        <f aca="false">3.48*10^(-4)</f>
+        <v>0.000348</v>
+      </c>
+      <c r="S19" s="37"/>
+      <c r="T19" s="37"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
+      <c r="M20" s="37"/>
+      <c r="N20" s="35" t="n">
+        <f aca="false">N$8*N9/(4*PI()*N$7*N$5)*(1-N$14)</f>
         <v>0.000665885867274975</v>
       </c>
-      <c r="O18" s="28" t="n">
-        <f aca="false">O8*O10/(4*PI()*O7*O6)</f>
+      <c r="O20" s="35" t="n">
+        <f aca="false">O$8*O9/(4*PI()*O$7*O$6)</f>
         <v>0.00106103295394597</v>
       </c>
-      <c r="P18" s="27" t="n">
-        <f aca="false">O18/N18</f>
+      <c r="P20" s="36" t="n">
+        <f aca="false">O20/N20</f>
         <v>1.59341563786008</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="29" t="n">
+      <c r="Q20" s="35" t="n">
+        <f aca="false">6.49*10^(-4)</f>
+        <v>0.000649</v>
+      </c>
+      <c r="R20" s="35" t="n">
+        <f aca="false">9.74*10^(-4)</f>
+        <v>0.000974</v>
+      </c>
+      <c r="S20" s="37" t="n">
+        <f aca="false">(Q20-N20)/Q20</f>
+        <v>-0.02601828547762</v>
+      </c>
+      <c r="T20" s="37" t="n">
+        <f aca="false">(R20-O20)/R20</f>
+        <v>-0.089356215550276</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9" t="n">
         <f aca="false">4*10^(-4)</f>
         <v>0.0004</v>
       </c>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="9" t="n">
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9" t="n">
         <f aca="false">3*10^(-4)</f>
         <v>0.0003</v>
       </c>
-      <c r="K19" s="29" t="n">
+      <c r="K21" s="9" t="n">
         <f aca="false">7.2*10^(-4)</f>
         <v>0.00072</v>
       </c>
-      <c r="L19" s="27" t="n">
-        <f aca="false">K19/J19</f>
+      <c r="L21" s="38" t="n">
+        <f aca="false">K21/J21</f>
         <v>2.4</v>
       </c>
-      <c r="N19" s="9"/>
-      <c r="O19" s="29" t="n">
+      <c r="N21" s="9"/>
+      <c r="O21" s="9" t="n">
         <f aca="false">4*10^(-4)</f>
         <v>0.0004</v>
       </c>
-      <c r="P19" s="29"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="K20" s="0" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="J21" s="0" t="n">
-        <f aca="false">J18/J19</f>
-        <v>1.89470170347494</v>
-      </c>
-      <c r="K21" s="0" t="n">
-        <f aca="false">K18/K19</f>
-        <v>2.91003996420862</v>
-      </c>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="6"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="J22" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="K22" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J23" s="0" t="n">
+        <f aca="false">J19/J21</f>
+        <v>1.89470170347494</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <f aca="false">K19/K21</f>
+        <v>2.91003996420862</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="J24" s="0" t="n">
         <f aca="false">1/KEStransparency!B30</f>
         <v>2.58790553719257</v>
       </c>
-      <c r="K22" s="0" t="n">
+      <c r="K24" s="0" t="n">
         <f aca="false">1/KEStransparency!B22</f>
         <v>1.75930577809311</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="J23" s="0" t="n">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="J25" s="0" t="n">
         <f aca="false">J16/J13</f>
         <v>1.4</v>
       </c>
-      <c r="K23" s="0" t="n">
+      <c r="K25" s="0" t="n">
         <f aca="false">K16/K13</f>
         <v>5.26588425976925</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0" t="s">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C28" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B27" s="31" t="n">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" s="39" t="n">
         <f aca="false">B16</f>
         <v>8.4</v>
       </c>
-      <c r="C27" s="31" t="n">
+      <c r="C29" s="39" t="n">
         <f aca="false">C16</f>
         <v>23.6964791689616</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="B28" s="31" t="n">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" s="39" t="n">
         <f aca="false">F16</f>
         <v>4</v>
       </c>
-      <c r="C28" s="31" t="n">
+      <c r="C30" s="39" t="n">
         <f aca="false">G16</f>
         <v>21.063537039077</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B29" s="31" t="n">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="39" t="n">
         <f aca="false">J16</f>
         <v>5.6</v>
       </c>
-      <c r="C29" s="31" t="n">
+      <c r="C31" s="39" t="n">
         <f aca="false">K16</f>
         <v>21.063537039077</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="B30" s="31" t="n">
-        <f aca="false">J17</f>
-        <v>6.3</v>
-      </c>
-      <c r="C30" s="31" t="n">
-        <f aca="false">K17</f>
-        <v>20.6</v>
-      </c>
-    </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="0" t="s">
-        <v>6</v>
+        <v>78</v>
+      </c>
+      <c r="B32" s="39" t="n">
+        <f aca="false">J18</f>
+        <v>6.3</v>
+      </c>
+      <c r="C32" s="39" t="n">
+        <f aca="false">K18</f>
+        <v>20.6</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B34" s="31" t="n">
-        <f aca="false">B18</f>
-        <v>0.00032740445436047</v>
-      </c>
-      <c r="C34" s="31" t="n">
-        <f aca="false">C18</f>
-        <v>0.00120249585297877</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="B35" s="31" t="n">
-        <f aca="false">F18</f>
-        <v>6.6314559621623E-005</v>
-      </c>
-      <c r="C35" s="31" t="n">
-        <f aca="false">G18</f>
-        <v>0.000465606394273379</v>
+      <c r="B35" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B36" s="31" t="n">
-        <f aca="false">J18</f>
-        <v>0.000568410511042483</v>
-      </c>
-      <c r="C36" s="31" t="n">
-        <f aca="false">K18</f>
-        <v>0.00209522877423021</v>
+        <v>75</v>
+      </c>
+      <c r="B36" s="39" t="n">
+        <f aca="false">B19</f>
+        <v>0.00032740445436047</v>
+      </c>
+      <c r="C36" s="39" t="n">
+        <f aca="false">C19</f>
+        <v>0.00120249585297877</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="B37" s="31" t="n">
-        <f aca="false">B36*KEStransparency!B30</f>
-        <v>0.000219641135610811</v>
-      </c>
-      <c r="C37" s="31" t="n">
-        <f aca="false">C36*KEStransparency!B22</f>
-        <v>0.0011909406541603</v>
+        <v>76</v>
+      </c>
+      <c r="B37" s="39" t="n">
+        <f aca="false">F19</f>
+        <v>6.6314559621623E-005</v>
+      </c>
+      <c r="C37" s="39" t="n">
+        <f aca="false">G19</f>
+        <v>0.000465606394273379</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="B38" s="31" t="n">
+        <v>77</v>
+      </c>
+      <c r="B38" s="39" t="n">
         <f aca="false">J19</f>
+        <v>0.000568410511042483</v>
+      </c>
+      <c r="C38" s="39" t="n">
+        <f aca="false">K19</f>
+        <v>0.00209522877423021</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" s="39" t="n">
+        <f aca="false">B38*KEStransparency!B30</f>
+        <v>0.000219641135610811</v>
+      </c>
+      <c r="C39" s="39" t="n">
+        <f aca="false">C38*KEStransparency!B22</f>
+        <v>0.0011909406541603</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" s="39" t="n">
+        <f aca="false">J21</f>
         <v>0.0003</v>
       </c>
-      <c r="C38" s="31" t="n">
-        <f aca="false">K19</f>
+      <c r="C40" s="39" t="n">
+        <f aca="false">K21</f>
         <v>0.00072</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="N1:T1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="N2:P2"/>
+    <mergeCell ref="Q2:R2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Etienne's edits after the reviews of Denis, Brent and David
</commit_message>
<xml_diff>
--- a/KES-MPS.xlsx
+++ b/KES-MPS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Brent" sheetId="1" state="visible" r:id="rId2"/>
@@ -218,19 +218,19 @@
     <t xml:space="preserve">Ratio</t>
   </si>
   <si>
+    <t xml:space="preserve">Res (mm) Perfect collimator </t>
+  </si>
+  <si>
     <t xml:space="preserve">Res (mm) Physical collimator</t>
   </si>
   <si>
-    <t xml:space="preserve">Res (mm) Perfect collimator </t>
-  </si>
-  <si>
     <t xml:space="preserve">Published Res (mm)</t>
   </si>
   <si>
+    <t xml:space="preserve">Eff Perfect collimator</t>
+  </si>
+  <si>
     <t xml:space="preserve">Eff Physical collimator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eff Perfect collimator</t>
   </si>
   <si>
     <t xml:space="preserve">Published eff</t>
@@ -423,7 +423,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -516,10 +516,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -528,7 +524,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -536,15 +532,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -552,15 +540,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -569,10 +553,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -696,10 +676,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.168752234537004"/>
-          <c:y val="0.110856573705179"/>
-          <c:w val="0.715480872363246"/>
-          <c:h val="0.685358565737052"/>
+          <c:x val="0.168764302059497"/>
+          <c:y val="0.110867616296444"/>
+          <c:w val="0.71546052631579"/>
+          <c:h val="0.685327223827074"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -875,11 +855,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="84877201"/>
-        <c:axId val="26537259"/>
+        <c:axId val="35552367"/>
+        <c:axId val="92020503"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84877201"/>
+        <c:axId val="35552367"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -907,14 +887,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26537259"/>
+        <c:crossAx val="92020503"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="26537259"/>
+        <c:axId val="92020503"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -979,7 +959,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84877201"/>
+        <c:crossAx val="35552367"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1243,11 +1223,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="8445730"/>
-        <c:axId val="83949643"/>
+        <c:axId val="26714919"/>
+        <c:axId val="46612256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="8445730"/>
+        <c:axId val="26714919"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1275,14 +1255,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83949643"/>
+        <c:crossAx val="46612256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83949643"/>
+        <c:axId val="46612256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1347,7 +1327,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8445730"/>
+        <c:crossAx val="26714919"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1414,9 +1394,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>462600</xdr:colOff>
+      <xdr:colOff>462240</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>50040</xdr:rowOff>
+      <xdr:rowOff>49680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1430,7 +1410,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9781560" y="0"/>
-          <a:ext cx="2030760" cy="2976120"/>
+          <a:ext cx="2030400" cy="2975760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1451,9 +1431,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>351360</xdr:colOff>
+      <xdr:colOff>351000</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>18000</xdr:rowOff>
+      <xdr:rowOff>17640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1467,7 +1447,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7571520" y="56160"/>
-          <a:ext cx="2325600" cy="2887920"/>
+          <a:ext cx="2325240" cy="2887560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1488,9 +1468,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>281160</xdr:colOff>
+      <xdr:colOff>280800</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>60120</xdr:rowOff>
+      <xdr:rowOff>59760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1504,7 +1484,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="173880" y="4492080"/>
-          <a:ext cx="3998880" cy="4996440"/>
+          <a:ext cx="3998520" cy="4996080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1525,9 +1505,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>572760</xdr:colOff>
+      <xdr:colOff>572400</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>85680</xdr:rowOff>
+      <xdr:rowOff>85320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1541,7 +1521,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11964960" y="474480"/>
-          <a:ext cx="4167000" cy="1886760"/>
+          <a:ext cx="4166640" cy="1886400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1562,9 +1542,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>361440</xdr:colOff>
+      <xdr:colOff>361080</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>135720</xdr:rowOff>
+      <xdr:rowOff>135360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1578,7 +1558,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4733640" y="4820400"/>
-          <a:ext cx="4572360" cy="3768120"/>
+          <a:ext cx="4572000" cy="3767760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1599,9 +1579,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>74880</xdr:colOff>
+      <xdr:colOff>74520</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>59400</xdr:rowOff>
+      <xdr:rowOff>59040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1615,7 +1595,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9942840" y="4930920"/>
-          <a:ext cx="4488480" cy="3744000"/>
+          <a:ext cx="4488120" cy="3743640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1641,9 +1621,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>519480</xdr:colOff>
+      <xdr:colOff>519120</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>50040</xdr:rowOff>
+      <xdr:rowOff>49680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1657,7 +1637,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5666760" y="0"/>
-          <a:ext cx="2050920" cy="2976120"/>
+          <a:ext cx="2050560" cy="2975760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1678,9 +1658,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>231840</xdr:colOff>
+      <xdr:colOff>231480</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>124560</xdr:rowOff>
+      <xdr:rowOff>124200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1694,7 +1674,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3911760" y="0"/>
-          <a:ext cx="2315520" cy="2887920"/>
+          <a:ext cx="2315160" cy="2887560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1715,9 +1695,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>116640</xdr:colOff>
+      <xdr:colOff>116280</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>28080</xdr:rowOff>
+      <xdr:rowOff>27720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1731,7 +1711,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7958520" y="416880"/>
-          <a:ext cx="4167000" cy="1886760"/>
+          <a:ext cx="4166640" cy="1886400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1757,9 +1737,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>131400</xdr:colOff>
+      <xdr:colOff>131040</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>15840</xdr:rowOff>
+      <xdr:rowOff>15480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1773,7 +1753,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8138880" y="3657600"/>
-          <a:ext cx="4160880" cy="1884960"/>
+          <a:ext cx="4160520" cy="1884600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1794,9 +1774,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>299160</xdr:colOff>
+      <xdr:colOff>298800</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>153720</xdr:rowOff>
+      <xdr:rowOff>153360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1810,7 +1790,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14210280" y="30960"/>
-          <a:ext cx="2321280" cy="2886120"/>
+          <a:ext cx="2320920" cy="2885760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1830,9 +1810,9 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>554040</xdr:colOff>
+      <xdr:colOff>554400</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>2520</xdr:rowOff>
+      <xdr:rowOff>2880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
@@ -1846,8 +1826,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4835520" y="4554000"/>
-        <a:ext cx="5034240" cy="3614040"/>
+        <a:off x="4835880" y="4554360"/>
+        <a:ext cx="5033880" cy="3613680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1862,7 +1842,7 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>4320</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>87480</xdr:rowOff>
+      <xdr:rowOff>87840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
@@ -1876,8 +1856,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10707120" y="4638960"/>
-        <a:ext cx="5756040" cy="3240720"/>
+        <a:off x="10707120" y="4639320"/>
+        <a:ext cx="5756040" cy="3240360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2862,7 +2842,7 @@
   </sheetPr>
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
     </sheetView>
   </sheetViews>
@@ -3146,8 +3126,8 @@
   </sheetPr>
   <dimension ref="A1:T40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T20" activeCellId="0" sqref="T20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T19" activeCellId="0" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3200,11 +3180,11 @@
       </c>
       <c r="K2" s="22"/>
       <c r="L2" s="22"/>
-      <c r="N2" s="23" t="s">
+      <c r="N2" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
       <c r="Q2" s="3" t="s">
         <v>61</v>
       </c>
@@ -3725,248 +3705,259 @@
       <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
       <c r="R15" s="6"/>
-      <c r="S15" s="6"/>
       <c r="T15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="25" t="n">
+      <c r="B16" s="23"/>
+      <c r="C16" s="24" t="n">
+        <f aca="false">C9*(1+C$4/C$6)</f>
+        <v>13.5</v>
+      </c>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="24" t="n">
+        <f aca="false">G9*(1+G$4/G$6)</f>
+        <v>12</v>
+      </c>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="24" t="n">
+        <f aca="false">K9*(1+K$4/K$6)</f>
+        <v>12</v>
+      </c>
+      <c r="L16" s="23"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="24" t="n">
+        <f aca="false">N9*(1+N4/N5)</f>
+        <v>14.52</v>
+      </c>
+      <c r="O16" s="24" t="n">
+        <f aca="false">O9*(1+O$4/O$6)</f>
+        <v>13.5</v>
+      </c>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="26" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="R16" s="26" t="n">
+        <v>12</v>
+      </c>
+      <c r="S16" s="26" t="n">
+        <f aca="false">(Q16-N16)/Q16</f>
+        <v>0.354666666666667</v>
+      </c>
+      <c r="T16" s="26" t="n">
+        <f aca="false">(R16-O16)/R16</f>
+        <v>-0.125</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="24" t="n">
         <f aca="false">B10*(1+B4/B5)</f>
         <v>8.4</v>
       </c>
-      <c r="C16" s="25" t="n">
+      <c r="C17" s="24" t="n">
         <f aca="false">C10*(1+C$4/C$6)</f>
         <v>23.6964791689616</v>
       </c>
-      <c r="D16" s="25" t="n">
-        <f aca="false">C16/B16</f>
+      <c r="D17" s="24" t="n">
+        <f aca="false">C17/B17</f>
         <v>2.82100942487638</v>
       </c>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25" t="n">
+      <c r="E17" s="24"/>
+      <c r="F17" s="24" t="n">
         <f aca="false">F10*(1+F4/F5)</f>
         <v>4</v>
       </c>
-      <c r="G16" s="25" t="n">
+      <c r="G17" s="24" t="n">
         <f aca="false">G10*(1+G$4/G$6)</f>
         <v>21.063537039077</v>
       </c>
-      <c r="H16" s="25" t="n">
-        <f aca="false">G16/F16</f>
+      <c r="H17" s="24" t="n">
+        <f aca="false">G17/F17</f>
         <v>5.26588425976925</v>
       </c>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25" t="n">
+      <c r="I17" s="24"/>
+      <c r="J17" s="24" t="n">
         <f aca="false">J10*(1+J4/J5)</f>
         <v>5.6</v>
       </c>
-      <c r="K16" s="25" t="n">
+      <c r="K17" s="24" t="n">
         <f aca="false">K10*(1+K$4/K$6)</f>
         <v>21.063537039077</v>
       </c>
-      <c r="L16" s="25" t="n">
-        <f aca="false">K16/J16</f>
+      <c r="L17" s="24" t="n">
+        <f aca="false">K17/J17</f>
         <v>3.76134589983518</v>
       </c>
-      <c r="M16" s="26"/>
-      <c r="N16" s="25" t="n">
-        <f aca="false">N10*(1+N4/N5)</f>
-        <v>14.52</v>
-      </c>
-      <c r="O16" s="25" t="n">
+      <c r="M17" s="27"/>
+      <c r="O17" s="24" t="n">
         <f aca="false">O10*(1+O$4/O$6)</f>
         <v>23.6964791689616</v>
       </c>
-      <c r="P16" s="25" t="n">
-        <f aca="false">O16/N16</f>
+      <c r="P17" s="24" t="n">
+        <f aca="false">O17/N16</f>
         <v>1.63198892348221</v>
       </c>
-      <c r="Q16" s="27" t="n">
-        <v>22.5</v>
-      </c>
-      <c r="R16" s="27" t="n">
+      <c r="R17" s="26" t="n">
         <v>19.3</v>
       </c>
-      <c r="S16" s="27" t="n">
-        <f aca="false">(Q16-N16)/Q16</f>
-        <v>0.354666666666667</v>
-      </c>
-      <c r="T16" s="27" t="n">
-        <f aca="false">(R16-O16)/R16</f>
+      <c r="S17" s="6"/>
+      <c r="T17" s="26" t="n">
+        <f aca="false">(R17-O17)/R17</f>
         <v>-0.227796848132727</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="25" t="n">
-        <f aca="false">C9*(1+C$4/C$6)</f>
-        <v>13.5</v>
-      </c>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="25" t="n">
-        <f aca="false">G9*(1+G$4/G$6)</f>
-        <v>12</v>
-      </c>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="25" t="n">
-        <f aca="false">K9*(1+K$4/K$6)</f>
-        <v>12</v>
-      </c>
-      <c r="L17" s="24"/>
-      <c r="M17" s="28"/>
-      <c r="N17" s="24"/>
-      <c r="O17" s="25" t="n">
-        <f aca="false">O9*(1+O$4/O$6)</f>
-        <v>13.5</v>
-      </c>
-      <c r="P17" s="24"/>
-      <c r="Q17" s="27"/>
-      <c r="R17" s="27" t="n">
-        <v>12</v>
-      </c>
-      <c r="S17" s="27"/>
-      <c r="T17" s="27" t="n">
-        <f aca="false">(R17-O17)/R17</f>
-        <v>-0.125</v>
-      </c>
-    </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="30" t="n">
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8" t="n">
         <v>6.3</v>
       </c>
-      <c r="K18" s="30" t="n">
+      <c r="K18" s="8" t="n">
         <v>20.6</v>
       </c>
-      <c r="L18" s="31" t="n">
+      <c r="L18" s="28" t="n">
         <f aca="false">K18/J18</f>
         <v>3.26984126984127</v>
       </c>
-      <c r="M18" s="32"/>
-      <c r="Q18" s="33"/>
-      <c r="R18" s="33"/>
-      <c r="S18" s="33"/>
-      <c r="T18" s="33"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="B19" s="35" t="n">
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="30"/>
+      <c r="M19" s="30"/>
+      <c r="N19" s="31" t="n">
+        <f aca="false">N$8*N9/(4*PI()*N$7*N$5)*(1-N$14)</f>
+        <v>0.000665885867274975</v>
+      </c>
+      <c r="O19" s="31" t="n">
+        <f aca="false">O$8*O9/(4*PI()*O$7*O$6)</f>
+        <v>0.00106103295394597</v>
+      </c>
+      <c r="P19" s="32" t="n">
+        <f aca="false">O19/N19</f>
+        <v>1.59341563786008</v>
+      </c>
+      <c r="Q19" s="31" t="n">
+        <f aca="false">6.49*10^(-4)</f>
+        <v>0.000649</v>
+      </c>
+      <c r="R19" s="31" t="n">
+        <f aca="false">9.74*10^(-4)</f>
+        <v>0.000974</v>
+      </c>
+      <c r="S19" s="30" t="n">
+        <f aca="false">(Q19-N19)/Q19</f>
+        <v>-0.02601828547762</v>
+      </c>
+      <c r="T19" s="30" t="n">
+        <f aca="false">(R19-O19)/R19</f>
+        <v>-0.089356215550276</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="31" t="n">
         <f aca="false">B8*B10/(4*PI()*B7*B5)*(1-B14)</f>
         <v>0.00032740445436047</v>
       </c>
-      <c r="C19" s="35" t="n">
+      <c r="C20" s="31" t="n">
         <f aca="false">C8*C10/(4*PI()*C7*C6)</f>
         <v>0.00120249585297877</v>
       </c>
-      <c r="D19" s="36" t="n">
-        <f aca="false">C19/B19</f>
+      <c r="D20" s="32" t="n">
+        <f aca="false">C20/B20</f>
         <v>3.67281457831</v>
       </c>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35" t="n">
+      <c r="E20" s="31"/>
+      <c r="F20" s="31" t="n">
         <f aca="false">F8*F10/(4*PI()*F7*F5)*(1-F14)</f>
         <v>6.6314559621623E-005</v>
       </c>
-      <c r="G19" s="35" t="n">
+      <c r="G20" s="31" t="n">
         <f aca="false">G8*G10/(4*PI()*G7*G6)</f>
         <v>0.000465606394273379</v>
       </c>
-      <c r="H19" s="36" t="n">
-        <f aca="false">G19/F19</f>
+      <c r="H20" s="32" t="n">
+        <f aca="false">G20/F20</f>
         <v>7.02117901302567</v>
       </c>
-      <c r="I19" s="35"/>
-      <c r="J19" s="35" t="n">
+      <c r="I20" s="31"/>
+      <c r="J20" s="31" t="n">
         <f aca="false">J8*J10/(4*PI()*J7*J5)*(1-J14)</f>
         <v>0.000568410511042483</v>
       </c>
-      <c r="K19" s="35" t="n">
+      <c r="K20" s="31" t="n">
         <f aca="false">K8*K10/(4*PI()*K7*K6)</f>
         <v>0.00209522877423021</v>
       </c>
-      <c r="L19" s="36" t="n">
-        <f aca="false">K19/J19</f>
+      <c r="L20" s="32" t="n">
+        <f aca="false">K20/J20</f>
         <v>3.68611898183847</v>
       </c>
-      <c r="M19" s="37"/>
-      <c r="N19" s="35"/>
-      <c r="O19" s="35"/>
-      <c r="P19" s="36"/>
-      <c r="Q19" s="35" t="n">
-        <f aca="false">3.4*10^(-4)</f>
-        <v>0.00034</v>
-      </c>
-      <c r="R19" s="35" t="n">
-        <f aca="false">3.48*10^(-4)</f>
-        <v>0.000348</v>
-      </c>
-      <c r="S19" s="37"/>
-      <c r="T19" s="37"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="37"/>
-      <c r="L20" s="37"/>
-      <c r="M20" s="37"/>
-      <c r="N20" s="35" t="n">
-        <f aca="false">N$8*N9/(4*PI()*N$7*N$5)*(1-N$14)</f>
-        <v>0.000665885867274975</v>
-      </c>
-      <c r="O20" s="35" t="n">
-        <f aca="false">O$8*O9/(4*PI()*O$7*O$6)</f>
-        <v>0.00106103295394597</v>
-      </c>
-      <c r="P20" s="36" t="n">
+      <c r="M20" s="30"/>
+      <c r="N20" s="31" t="n">
+        <f aca="false">N19*KEStransparency!B38</f>
+        <v>0.000376127521434265</v>
+      </c>
+      <c r="O20" s="31" t="n">
+        <f aca="false">O19*KEStransparency!B22</f>
+        <v>0.000603097521282521</v>
+      </c>
+      <c r="P20" s="32" t="n">
         <f aca="false">O20/N20</f>
-        <v>1.59341563786008</v>
-      </c>
-      <c r="Q20" s="35" t="n">
-        <f aca="false">6.49*10^(-4)</f>
-        <v>0.000649</v>
-      </c>
-      <c r="R20" s="35" t="n">
-        <f aca="false">9.74*10^(-4)</f>
-        <v>0.000974</v>
-      </c>
-      <c r="S20" s="37" t="n">
+        <v>1.603438958635</v>
+      </c>
+      <c r="Q20" s="31" t="n">
+        <f aca="false">6.61*10^(-4)</f>
+        <v>0.000661</v>
+      </c>
+      <c r="R20" s="31" t="n">
+        <f aca="false">1.03*10^(-3)</f>
+        <v>0.00103</v>
+      </c>
+      <c r="S20" s="30" t="n">
         <f aca="false">(Q20-N20)/Q20</f>
-        <v>-0.02601828547762</v>
-      </c>
-      <c r="T20" s="37" t="n">
+        <v>0.430971979675848</v>
+      </c>
+      <c r="T20" s="30" t="n">
         <f aca="false">(R20-O20)/R20</f>
-        <v>-0.089356215550276</v>
+        <v>0.4144684259393</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3992,7 +3983,7 @@
         <f aca="false">7.2*10^(-4)</f>
         <v>0.00072</v>
       </c>
-      <c r="L21" s="38" t="n">
+      <c r="L21" s="33" t="n">
         <f aca="false">K21/J21</f>
         <v>2.4</v>
       </c>
@@ -4023,11 +4014,11 @@
         <v>71</v>
       </c>
       <c r="J23" s="0" t="n">
-        <f aca="false">J19/J21</f>
+        <f aca="false">J20/J21</f>
         <v>1.89470170347494</v>
       </c>
       <c r="K23" s="0" t="n">
-        <f aca="false">K19/K21</f>
+        <f aca="false">K20/K21</f>
         <v>2.91003996420862</v>
       </c>
     </row>
@@ -4049,11 +4040,11 @@
         <v>73</v>
       </c>
       <c r="J25" s="0" t="n">
-        <f aca="false">J16/J13</f>
+        <f aca="false">J17/J13</f>
         <v>1.4</v>
       </c>
       <c r="K25" s="0" t="n">
-        <f aca="false">K16/K13</f>
+        <f aca="false">K17/K13</f>
         <v>5.26588425976925</v>
       </c>
     </row>
@@ -4074,12 +4065,12 @@
       <c r="A29" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="B29" s="39" t="n">
-        <f aca="false">B16</f>
+      <c r="B29" s="34" t="n">
+        <f aca="false">B17</f>
         <v>8.4</v>
       </c>
-      <c r="C29" s="39" t="n">
-        <f aca="false">C16</f>
+      <c r="C29" s="34" t="n">
+        <f aca="false">C17</f>
         <v>23.6964791689616</v>
       </c>
     </row>
@@ -4087,12 +4078,12 @@
       <c r="A30" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="B30" s="39" t="n">
-        <f aca="false">F16</f>
+      <c r="B30" s="34" t="n">
+        <f aca="false">F17</f>
         <v>4</v>
       </c>
-      <c r="C30" s="39" t="n">
-        <f aca="false">G16</f>
+      <c r="C30" s="34" t="n">
+        <f aca="false">G17</f>
         <v>21.063537039077</v>
       </c>
     </row>
@@ -4100,12 +4091,12 @@
       <c r="A31" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="B31" s="39" t="n">
-        <f aca="false">J16</f>
+      <c r="B31" s="34" t="n">
+        <f aca="false">J17</f>
         <v>5.6</v>
       </c>
-      <c r="C31" s="39" t="n">
-        <f aca="false">K16</f>
+      <c r="C31" s="34" t="n">
+        <f aca="false">K17</f>
         <v>21.063537039077</v>
       </c>
     </row>
@@ -4113,11 +4104,11 @@
       <c r="A32" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="B32" s="39" t="n">
+      <c r="B32" s="34" t="n">
         <f aca="false">J18</f>
         <v>6.3</v>
       </c>
-      <c r="C32" s="39" t="n">
+      <c r="C32" s="34" t="n">
         <f aca="false">K18</f>
         <v>20.6</v>
       </c>
@@ -4139,12 +4130,12 @@
       <c r="A36" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="B36" s="39" t="n">
-        <f aca="false">B19</f>
+      <c r="B36" s="34" t="n">
+        <f aca="false">B20</f>
         <v>0.00032740445436047</v>
       </c>
-      <c r="C36" s="39" t="n">
-        <f aca="false">C19</f>
+      <c r="C36" s="34" t="n">
+        <f aca="false">C20</f>
         <v>0.00120249585297877</v>
       </c>
     </row>
@@ -4152,12 +4143,12 @@
       <c r="A37" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="B37" s="39" t="n">
-        <f aca="false">F19</f>
+      <c r="B37" s="34" t="n">
+        <f aca="false">F20</f>
         <v>6.6314559621623E-005</v>
       </c>
-      <c r="C37" s="39" t="n">
-        <f aca="false">G19</f>
+      <c r="C37" s="34" t="n">
+        <f aca="false">G20</f>
         <v>0.000465606394273379</v>
       </c>
     </row>
@@ -4165,12 +4156,12 @@
       <c r="A38" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="B38" s="39" t="n">
-        <f aca="false">J19</f>
+      <c r="B38" s="34" t="n">
+        <f aca="false">J20</f>
         <v>0.000568410511042483</v>
       </c>
-      <c r="C38" s="39" t="n">
-        <f aca="false">K19</f>
+      <c r="C38" s="34" t="n">
+        <f aca="false">K20</f>
         <v>0.00209522877423021</v>
       </c>
     </row>
@@ -4178,11 +4169,11 @@
       <c r="A39" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="B39" s="39" t="n">
+      <c r="B39" s="34" t="n">
         <f aca="false">B38*KEStransparency!B30</f>
         <v>0.000219641135610811</v>
       </c>
-      <c r="C39" s="39" t="n">
+      <c r="C39" s="34" t="n">
         <f aca="false">C38*KEStransparency!B22</f>
         <v>0.0011909406541603</v>
       </c>
@@ -4191,11 +4182,11 @@
       <c r="A40" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="B40" s="39" t="n">
+      <c r="B40" s="34" t="n">
         <f aca="false">J21</f>
         <v>0.0003</v>
       </c>
-      <c r="C40" s="39" t="n">
+      <c r="C40" s="34" t="n">
         <f aca="false">K21</f>
         <v>0.00072</v>
       </c>

</xml_diff>

<commit_message>
minor modifications during paper reviewing to make the status on the results remaining to be finalized
</commit_message>
<xml_diff>
--- a/KES-MPS.xlsx
+++ b/KES-MPS.xlsx
@@ -5,14 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Brent" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Lin" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="AbsoluteEfficiency" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="KEStransparency" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="AllTogether" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="KEStransparency" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="AllTogether" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="76">
   <si>
     <t xml:space="preserve">Simulation results</t>
   </si>
@@ -129,21 +127,6 @@
   </si>
   <si>
     <t xml:space="preserve">KES, TOF, 1 MeV &lt; E &lt; 8 MeV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geometrical calculations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MPS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lin. Coll. Eff (relative)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Detection efficiency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Efficaicté KES publiée</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.physics.nist.gov/PhysRefData/Xcom/html/xcom1.html</t>
@@ -676,10 +659,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.168764302059497"/>
-          <c:y val="0.110867616296444"/>
-          <c:w val="0.71546052631579"/>
-          <c:h val="0.685327223827074"/>
+          <c:x val="0.168788442282935"/>
+          <c:y val="0.110889708080104"/>
+          <c:w val="0.715419825489916"/>
+          <c:h val="0.685264521271296"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -855,11 +838,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="35552367"/>
-        <c:axId val="92020503"/>
+        <c:axId val="40510485"/>
+        <c:axId val="76607678"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="35552367"/>
+        <c:axId val="40510485"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -887,14 +870,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92020503"/>
+        <c:crossAx val="76607678"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92020503"/>
+        <c:axId val="76607678"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -959,7 +942,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35552367"/>
+        <c:crossAx val="40510485"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1223,11 +1206,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="26714919"/>
-        <c:axId val="46612256"/>
+        <c:axId val="86139981"/>
+        <c:axId val="40592378"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="26714919"/>
+        <c:axId val="86139981"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1255,14 +1238,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46612256"/>
+        <c:crossAx val="40592378"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46612256"/>
+        <c:axId val="40592378"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1327,7 +1310,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26714919"/>
+        <c:crossAx val="86139981"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1394,9 +1377,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>462240</xdr:colOff>
+      <xdr:colOff>461520</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>49680</xdr:rowOff>
+      <xdr:rowOff>48960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1410,7 +1393,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9781560" y="0"/>
-          <a:ext cx="2030400" cy="2975760"/>
+          <a:ext cx="2029680" cy="2975040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1431,9 +1414,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>351000</xdr:colOff>
+      <xdr:colOff>350280</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>17640</xdr:rowOff>
+      <xdr:rowOff>16920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1447,7 +1430,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7571520" y="56160"/>
-          <a:ext cx="2325240" cy="2887560"/>
+          <a:ext cx="2324520" cy="2886840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1468,9 +1451,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>280800</xdr:colOff>
+      <xdr:colOff>280080</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>59760</xdr:rowOff>
+      <xdr:rowOff>59040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1484,7 +1467,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="173880" y="4492080"/>
-          <a:ext cx="3998520" cy="4996080"/>
+          <a:ext cx="3997800" cy="4995360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1505,9 +1488,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>572400</xdr:colOff>
+      <xdr:colOff>571680</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>85320</xdr:rowOff>
+      <xdr:rowOff>84600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1521,7 +1504,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11964960" y="474480"/>
-          <a:ext cx="4166640" cy="1886400"/>
+          <a:ext cx="4165920" cy="1885680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1542,9 +1525,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>361080</xdr:colOff>
+      <xdr:colOff>360360</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>135360</xdr:rowOff>
+      <xdr:rowOff>134640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1558,7 +1541,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4733640" y="4820400"/>
-          <a:ext cx="4572000" cy="3767760"/>
+          <a:ext cx="4571280" cy="3767040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1579,9 +1562,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>74520</xdr:colOff>
+      <xdr:colOff>73800</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>59040</xdr:rowOff>
+      <xdr:rowOff>58320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1595,7 +1578,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9942840" y="4930920"/>
-          <a:ext cx="4488120" cy="3743640"/>
+          <a:ext cx="4487400" cy="3742920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1612,201 +1595,6 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>272520</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>519120</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>49680</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Image 1" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5666760" y="0"/>
-          <a:ext cx="2050560" cy="2975760"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>321480</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>231480</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>124200</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Image 2" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId2"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3911760" y="0"/>
-          <a:ext cx="2315160" cy="2887560"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>159120</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>91800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>116280</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>27720</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Image 5" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId3"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7958520" y="416880"/>
-          <a:ext cx="4166640" cy="1886400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>34560</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>131040</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>15480</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Image 5" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8138880" y="3657600"/>
-          <a:ext cx="4160520" cy="1884600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>416520</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>30960</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>298800</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>153360</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Image 2" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId2"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14210280" y="30960"/>
-          <a:ext cx="2320920" cy="2885760"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
@@ -1816,18 +1604,18 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>200160</xdr:colOff>
+      <xdr:colOff>199440</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>40320</xdr:rowOff>
+      <xdr:rowOff>39600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="11" name=""/>
+        <xdr:cNvPr id="6" name=""/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="4835880" y="4554360"/>
-        <a:ext cx="5033880" cy="3613680"/>
+        <a:ext cx="5033160" cy="3612960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1846,18 +1634,18 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>70920</xdr:colOff>
+      <xdr:colOff>70200</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>77040</xdr:rowOff>
+      <xdr:rowOff>76320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="12" name=""/>
+        <xdr:cNvPr id="7" name=""/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="10707120" y="4639320"/>
-        <a:ext cx="5756040" cy="3240360"/>
+        <a:ext cx="5755320" cy="3239640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1877,7 +1665,7 @@
   </sheetPr>
   <dimension ref="A2:X29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -2387,463 +2175,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="3.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
-      <c r="B3" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="6" t="n">
-        <v>300</v>
-      </c>
-      <c r="C4" s="6" t="n">
-        <v>300</v>
-      </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="6" t="n">
-        <v>200</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="6" t="n">
-        <v>300</v>
-      </c>
-      <c r="C6" s="6" t="n">
-        <v>300</v>
-      </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="6" t="n">
-        <f aca="false">B4+B5+B6</f>
-        <v>800</v>
-      </c>
-      <c r="C7" s="6" t="n">
-        <f aca="false">SUM(C4:C6)</f>
-        <v>600</v>
-      </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="C8" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="6" t="n">
-        <f aca="false">B9/(B8+B9)</f>
-        <v>0.5</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="6" t="n">
-        <f aca="false">B5*B10</f>
-        <v>100</v>
-      </c>
-      <c r="C11" s="6" t="n">
-        <v>40</v>
-      </c>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="6" t="n">
-        <f aca="false">B8*(1+B4/B5)</f>
-        <v>5</v>
-      </c>
-      <c r="C12" s="6" t="n">
-        <f aca="false">C8*(1+C4/C6)</f>
-        <v>12</v>
-      </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="9" t="n">
-        <f aca="false">B8*(1-B10)/(B7*B5)</f>
-        <v>6.25E-006</v>
-      </c>
-      <c r="C13" s="9" t="e">
-        <f aca="false">C3*C2/(4*PI()*C1*#REF!)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="6" t="e">
-        <f aca="false">C13/B13</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A18:D18"/>
-  </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
-  </headerFooter>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:G27"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.61"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="6" t="n">
-        <v>320</v>
-      </c>
-      <c r="C3" s="6" t="n">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="6" t="n">
-        <v>190</v>
-      </c>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="6" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="6" t="n">
-        <f aca="false">B3+B4+B5</f>
-        <v>510</v>
-      </c>
-      <c r="C6" s="6" t="n">
-        <f aca="false">SUM(C3:C5)</f>
-        <v>450</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="6" t="n">
-        <v>3</v>
-      </c>
-      <c r="C8" s="6" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <f aca="false">B8+B9</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <f aca="false">B11/B10</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="6" t="n">
-        <f aca="false">B9/(B8+B9)</f>
-        <v>0.4</v>
-      </c>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="6" t="n">
-        <f aca="false">B4*B13</f>
-        <v>76</v>
-      </c>
-      <c r="C14" s="6" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="6" t="n">
-        <f aca="false">B8*(1+B3/B4)</f>
-        <v>8.05263157894737</v>
-      </c>
-      <c r="C15" s="6" t="n">
-        <f aca="false">C8*(1+C3/C5)</f>
-        <v>13.5</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="9" t="n">
-        <f aca="false">B8*B7/(4*PI()*B6*B4)*(1-B13)</f>
-        <v>0.000147821928568324</v>
-      </c>
-      <c r="C16" s="9" t="n">
-        <f aca="false">C8*C7/(4*PI()*C6*C5)</f>
-        <v>0.00106103295394597</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="9" t="n">
-        <f aca="false">B12*B16</f>
-        <v>0.000739109642841619</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="6" t="n">
-        <f aca="false">C16/B17</f>
-        <v>1.43555555555556</v>
-      </c>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F26" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="G26" s="0" t="n">
-        <f aca="false">4*10^(-4)</f>
-        <v>0.0004</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="0" t="n">
-        <f aca="false">100*3/(4*PI()*B6^2)</f>
-        <v>9.17848576077828E-005</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B89" activeCellId="0" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2857,17 +2192,17 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F1" s="16" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="17" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B3" s="18" t="n">
         <f aca="false">1.93*10</f>
@@ -2880,13 +2215,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
@@ -2909,12 +2244,12 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>40</v>
@@ -2922,7 +2257,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>63</v>
@@ -2930,7 +2265,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="19" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B10" s="0" t="n">
         <f aca="false">B8/2/TAN(B9*PI()/180)</f>
@@ -2939,7 +2274,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B13" s="0" t="n">
         <f aca="false">LN(2)/(C5*TAN(B9*PI()/180))*10</f>
@@ -2948,12 +2283,12 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="20" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>7.4</v>
@@ -2961,13 +2296,13 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="19" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2984,7 +2319,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>3</v>
@@ -2992,7 +2327,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B22" s="0" t="n">
         <f aca="false">1-EXP(-C19*B21)</f>
@@ -3001,12 +2336,12 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="20" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>4.51</v>
@@ -3014,13 +2349,13 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="19" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3037,7 +2372,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>3</v>
@@ -3045,7 +2380,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B30" s="0" t="n">
         <f aca="false">1-EXP(-C27*B29)</f>
@@ -3054,12 +2389,12 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="20" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>7.13</v>
@@ -3067,13 +2402,13 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="19" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3090,7 +2425,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>3</v>
@@ -3098,7 +2433,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B38" s="0" t="n">
         <f aca="false">1-EXP(-C35*B37)</f>
@@ -3119,15 +2454,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:T40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T19" activeCellId="0" sqref="T19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N19" activeCellId="0" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3152,7 +2487,7 @@
       <c r="D1" s="21"/>
       <c r="E1" s="21"/>
       <c r="N1" s="22" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="O1" s="22"/>
       <c r="P1" s="22"/>
@@ -3164,33 +2499,33 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="22" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
       <c r="E2" s="2"/>
       <c r="F2" s="22" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G2" s="22"/>
       <c r="H2" s="22"/>
       <c r="I2" s="2"/>
       <c r="J2" s="22" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="K2" s="22"/>
       <c r="L2" s="22"/>
       <c r="N2" s="5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="R2" s="3"/>
       <c r="S2" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="T2" s="6"/>
     </row>
@@ -3203,7 +2538,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="1" t="s">
@@ -3213,7 +2548,7 @@
         <v>6</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="1" t="s">
@@ -3223,7 +2558,7 @@
         <v>6</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>5</v>
@@ -3232,7 +2567,7 @@
         <v>6</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>5</v>
@@ -3709,7 +3044,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="23" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B16" s="23"/>
       <c r="C16" s="24" t="n">
@@ -3758,7 +3093,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="23" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B17" s="24" t="n">
         <f aca="false">B10*(1+B4/B5)</f>
@@ -3818,7 +3153,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -3845,7 +3180,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="29" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B19" s="30"/>
       <c r="C19" s="30"/>
@@ -3890,7 +3225,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="29" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B20" s="31" t="n">
         <f aca="false">B8*B10/(4*PI()*B7*B5)*(1-B14)</f>
@@ -3902,7 +3237,7 @@
       </c>
       <c r="D20" s="32" t="n">
         <f aca="false">C20/B20</f>
-        <v>3.67281457831</v>
+        <v>3.67281457831001</v>
       </c>
       <c r="E20" s="31"/>
       <c r="F20" s="31" t="n">
@@ -3928,7 +3263,7 @@
       </c>
       <c r="L20" s="32" t="n">
         <f aca="false">K20/J20</f>
-        <v>3.68611898183847</v>
+        <v>3.68611898183848</v>
       </c>
       <c r="M20" s="30"/>
       <c r="N20" s="31" t="n">
@@ -3937,7 +3272,7 @@
       </c>
       <c r="O20" s="31" t="n">
         <f aca="false">O19*KEStransparency!B22</f>
-        <v>0.000603097521282521</v>
+        <v>0.00060309752128252</v>
       </c>
       <c r="P20" s="32" t="n">
         <f aca="false">O20/N20</f>
@@ -3957,12 +3292,12 @@
       </c>
       <c r="T20" s="30" t="n">
         <f aca="false">(R20-O20)/R20</f>
-        <v>0.4144684259393</v>
+        <v>0.414468425939301</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="9" t="n">
@@ -4000,18 +3335,18 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C22" s="19" t="s">
         <v>1</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="J23" s="0" t="n">
         <f aca="false">J20/J21</f>
@@ -4024,11 +3359,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="J24" s="0" t="n">
-        <f aca="false">1/KEStransparency!B30</f>
-        <v>2.58790553719257</v>
+        <v>67</v>
       </c>
       <c r="K24" s="0" t="n">
         <f aca="false">1/KEStransparency!B22</f>
@@ -4037,7 +3368,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="J25" s="0" t="n">
         <f aca="false">J17/J13</f>
@@ -4050,7 +3381,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="17" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4063,7 +3394,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B29" s="34" t="n">
         <f aca="false">B17</f>
@@ -4076,7 +3407,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B30" s="34" t="n">
         <f aca="false">F17</f>
@@ -4089,7 +3420,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B31" s="34" t="n">
         <f aca="false">J17</f>
@@ -4102,7 +3433,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B32" s="34" t="n">
         <f aca="false">J18</f>
@@ -4115,7 +3446,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4128,7 +3459,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B36" s="34" t="n">
         <f aca="false">B20</f>
@@ -4141,7 +3472,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B37" s="34" t="n">
         <f aca="false">F20</f>
@@ -4154,7 +3485,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B38" s="34" t="n">
         <f aca="false">J20</f>
@@ -4167,7 +3498,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B39" s="34" t="n">
         <f aca="false">B38*KEStransparency!B30</f>
@@ -4180,7 +3511,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B40" s="34" t="n">
         <f aca="false">J21</f>

</xml_diff>